<commit_message>
xlsx and invest dummy update
</commit_message>
<xml_diff>
--- a/Datei.xlsx
+++ b/Datei.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://horvathandpartners.sharepoint.com/sites/IFUA-IDEX.TAN.T55170/Freigegebene Dokumente/02_Munka/01_Projektmunka_IFUA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{86743A00-2BEF-4DB1-8E09-172417BF45B5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{46812FD0-6F85-4265-BD6F-F60C82E643E2}"/>
+  <xr:revisionPtr revIDLastSave="40" documentId="8_{86743A00-2BEF-4DB1-8E09-172417BF45B5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{20E40BB5-3356-42C2-BF77-F2780BA2133E}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="775" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="775" uniqueCount="289">
   <si>
     <t>Account ID</t>
   </si>
@@ -905,9 +905,6 @@
   </si>
   <si>
     <t>Amount, Usage, Duration</t>
-  </si>
-  <si>
-    <t>Usage, Duration, Null</t>
   </si>
 </sst>
 </file>
@@ -956,7 +953,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -967,6 +964,12 @@
       <patternFill patternType="solid">
         <fgColor indexed="9"/>
         <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1027,7 +1030,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -1094,193 +1097,12 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="27">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <fill>
         <patternFill>
@@ -2607,27 +2429,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L117"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B10" sqref="B10"/>
+      <selection pane="bottomRight" activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.45" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="9.88671875" style="25" customWidth="1"/>
-    <col min="2" max="2" width="46.33203125" style="25" customWidth="1"/>
-    <col min="3" max="3" width="17.21875" style="25" customWidth="1"/>
-    <col min="4" max="4" width="18.33203125" style="25" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.6640625" style="26" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.6640625" style="25" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.6640625" style="25" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.6640625" style="27" customWidth="1"/>
-    <col min="9" max="9" width="12.44140625" style="27" customWidth="1"/>
-    <col min="10" max="10" width="5.6640625" style="25" customWidth="1"/>
+    <col min="1" max="1" width="9.85546875" style="25" customWidth="1"/>
+    <col min="2" max="2" width="46.28515625" style="25" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" style="25" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" style="25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" style="26" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" style="25" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.7109375" style="25" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="41" style="27" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.42578125" style="27" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.7109375" style="25" customWidth="1"/>
     <col min="11" max="11" width="17" style="27" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="22.109375" style="27" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.140625" style="27" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="30" customFormat="1" ht="15" customHeight="1">
@@ -2668,7 +2490,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="17.399999999999999" customHeight="1">
+    <row r="2" spans="1:12" ht="17.45" customHeight="1">
       <c r="A2" s="13">
         <v>681100</v>
       </c>
@@ -2721,7 +2543,7 @@
         <v>Geschenk1</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="17.399999999999999" customHeight="1">
+    <row r="3" spans="1:12" ht="17.45" customHeight="1">
       <c r="A3" s="13">
         <v>681120</v>
       </c>
@@ -2774,7 +2596,7 @@
         <v>Geschenk</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="17.399999999999999" customHeight="1">
+    <row r="4" spans="1:12" ht="17.45" customHeight="1">
       <c r="A4" s="13">
         <v>661601</v>
       </c>
@@ -2827,7 +2649,7 @@
         <v>Geschenk2</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="17.399999999999999" customHeight="1">
+    <row r="5" spans="1:12" ht="17.45" customHeight="1">
       <c r="A5" s="13">
         <v>661602</v>
       </c>
@@ -2880,7 +2702,7 @@
         <v>Geschenk3</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="17.399999999999999" customHeight="1">
+    <row r="6" spans="1:12" ht="17.45" customHeight="1">
       <c r="A6" s="13">
         <v>603900</v>
       </c>
@@ -2933,7 +2755,7 @@
         <v>Aktivierung2</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="17.399999999999999" customHeight="1">
+    <row r="7" spans="1:12" ht="17.45" customHeight="1">
       <c r="A7" s="13">
         <v>603900</v>
       </c>
@@ -2986,7 +2808,7 @@
         <v>Aktivierung1</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="17.399999999999999" customHeight="1">
+    <row r="8" spans="1:12" ht="17.45" customHeight="1">
       <c r="A8" s="13">
         <v>603900</v>
       </c>
@@ -3014,7 +2836,7 @@
       </c>
       <c r="I8" s="28" t="str">
         <f>VLOOKUP(L8,'Logic ID'!$E:$G,3,0)</f>
-        <v>Amount, Usage, Null</v>
+        <v>Amount, Usage, Duration</v>
       </c>
       <c r="J8" s="20" t="s">
         <v>269</v>
@@ -3039,7 +2861,7 @@
         <v>Aktivierung3</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="17.399999999999999" customHeight="1">
+    <row r="9" spans="1:12" ht="17.45" customHeight="1">
       <c r="A9" s="13">
         <v>695800</v>
       </c>
@@ -3092,7 +2914,7 @@
         <v>Aktivierung2</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="17.399999999999999" customHeight="1">
+    <row r="10" spans="1:12" ht="17.45" customHeight="1">
       <c r="A10" s="13">
         <v>695800</v>
       </c>
@@ -3145,7 +2967,7 @@
         <v>Aktivierung1</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="17.399999999999999" customHeight="1">
+    <row r="11" spans="1:12" ht="17.45" customHeight="1">
       <c r="A11" s="13">
         <v>695800</v>
       </c>
@@ -3173,7 +2995,7 @@
       </c>
       <c r="I11" s="28" t="str">
         <f>VLOOKUP(L11,'Logic ID'!$E:$G,3,0)</f>
-        <v>Amount, Usage, Null</v>
+        <v>Amount, Usage, Duration</v>
       </c>
       <c r="J11" s="20" t="s">
         <v>269</v>
@@ -3198,7 +3020,7 @@
         <v>Aktivierung3</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="17.399999999999999" customHeight="1">
+    <row r="12" spans="1:12" ht="17.45" customHeight="1">
       <c r="A12" s="13">
         <v>681203</v>
       </c>
@@ -3251,7 +3073,7 @@
         <v>Aktivierung2</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="17.399999999999999" customHeight="1">
+    <row r="13" spans="1:12" ht="17.45" customHeight="1">
       <c r="A13" s="13">
         <v>681203</v>
       </c>
@@ -3304,7 +3126,7 @@
         <v>Aktivierung1</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="17.399999999999999" customHeight="1">
+    <row r="14" spans="1:12" ht="17.45" customHeight="1">
       <c r="A14" s="13">
         <v>681203</v>
       </c>
@@ -3332,7 +3154,7 @@
       </c>
       <c r="I14" s="28" t="str">
         <f>VLOOKUP(L14,'Logic ID'!$E:$G,3,0)</f>
-        <v>Amount, Usage, Null</v>
+        <v>Amount, Usage, Duration</v>
       </c>
       <c r="J14" s="20" t="s">
         <v>269</v>
@@ -3357,7 +3179,7 @@
         <v>Aktivierung3</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="17.399999999999999" customHeight="1">
+    <row r="15" spans="1:12" ht="17.45" customHeight="1">
       <c r="A15" s="13">
         <v>661603</v>
       </c>
@@ -3410,7 +3232,7 @@
         <v>Geschenk</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="17.399999999999999" customHeight="1">
+    <row r="16" spans="1:12" ht="17.45" customHeight="1">
       <c r="A16" s="13">
         <v>672200</v>
       </c>
@@ -3463,7 +3285,7 @@
         <v>Keine Aktivierung</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="17.399999999999999" customHeight="1">
+    <row r="17" spans="1:12" ht="17.45" customHeight="1">
       <c r="A17" s="13">
         <v>662100</v>
       </c>
@@ -3516,7 +3338,7 @@
         <v>Keine Aktivierung</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="17.399999999999999" customHeight="1">
+    <row r="18" spans="1:12" ht="17.45" customHeight="1">
       <c r="A18" s="13">
         <v>662201</v>
       </c>
@@ -3569,7 +3391,7 @@
         <v>Keine Aktivierung</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="17.399999999999999" customHeight="1">
+    <row r="19" spans="1:12" ht="17.45" customHeight="1">
       <c r="A19" s="13">
         <v>661700</v>
       </c>
@@ -3622,7 +3444,7 @@
         <v>Keine Aktivierung</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="17.399999999999999" customHeight="1">
+    <row r="20" spans="1:12" ht="17.45" customHeight="1">
       <c r="A20" s="13">
         <v>662300</v>
       </c>
@@ -3675,7 +3497,7 @@
         <v>Keine Aktivierung</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="17.399999999999999" customHeight="1">
+    <row r="21" spans="1:12" ht="17.45" customHeight="1">
       <c r="A21" s="13">
         <v>661703</v>
       </c>
@@ -3728,7 +3550,7 @@
         <v>Keine Aktivierung</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="17.399999999999999" customHeight="1">
+    <row r="22" spans="1:12" ht="17.45" customHeight="1">
       <c r="A22" s="13">
         <v>661710</v>
       </c>
@@ -3781,7 +3603,7 @@
         <v>Keine Aktivierung</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="17.399999999999999" customHeight="1">
+    <row r="23" spans="1:12" ht="17.45" customHeight="1">
       <c r="A23" s="13">
         <v>661708</v>
       </c>
@@ -3834,7 +3656,7 @@
         <v>Keine Aktivierung</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="17.399999999999999" customHeight="1">
+    <row r="24" spans="1:12" ht="17.45" customHeight="1">
       <c r="A24" s="13">
         <v>681150</v>
       </c>
@@ -3887,7 +3709,7 @@
         <v>WVDV1</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="17.399999999999999" customHeight="1">
+    <row r="25" spans="1:12" ht="17.45" customHeight="1">
       <c r="A25" s="13">
         <v>681150</v>
       </c>
@@ -3915,7 +3737,7 @@
       </c>
       <c r="I25" s="28" t="str">
         <f>VLOOKUP(L25,'Logic ID'!$E:$G,3,0)</f>
-        <v>Usage, Duration, Null</v>
+        <v>Amount, Usage, Duration</v>
       </c>
       <c r="J25" s="20" t="s">
         <v>271</v>
@@ -3940,7 +3762,7 @@
         <v>WVDV2</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="17.399999999999999" customHeight="1">
+    <row r="26" spans="1:12" ht="17.45" customHeight="1">
       <c r="A26" s="13">
         <v>673800</v>
       </c>
@@ -3993,7 +3815,7 @@
         <v>WVDV1</v>
       </c>
     </row>
-    <row r="27" spans="1:12" ht="17.399999999999999" customHeight="1">
+    <row r="27" spans="1:12" ht="17.45" customHeight="1">
       <c r="A27" s="13">
         <v>673800</v>
       </c>
@@ -4021,7 +3843,7 @@
       </c>
       <c r="I27" s="28" t="str">
         <f>VLOOKUP(L27,'Logic ID'!$E:$G,3,0)</f>
-        <v>Usage, Duration, Null</v>
+        <v>Amount, Usage, Duration</v>
       </c>
       <c r="J27" s="20" t="s">
         <v>271</v>
@@ -4046,7 +3868,7 @@
         <v>WVDV2</v>
       </c>
     </row>
-    <row r="28" spans="1:12" ht="17.399999999999999" customHeight="1">
+    <row r="28" spans="1:12" ht="17.45" customHeight="1">
       <c r="A28" s="13">
         <v>661200</v>
       </c>
@@ -4099,7 +3921,7 @@
         <v>Keine Aktivierung</v>
       </c>
     </row>
-    <row r="29" spans="1:12" ht="17.399999999999999" customHeight="1">
+    <row r="29" spans="1:12" ht="17.45" customHeight="1">
       <c r="A29" s="13">
         <v>681153</v>
       </c>
@@ -4152,7 +3974,7 @@
         <v>Keine Aktivierung</v>
       </c>
     </row>
-    <row r="30" spans="1:12" ht="17.399999999999999" customHeight="1">
+    <row r="30" spans="1:12" ht="17.45" customHeight="1">
       <c r="A30" s="13">
         <v>672201</v>
       </c>
@@ -4205,7 +4027,7 @@
         <v>Keine Aktivierung</v>
       </c>
     </row>
-    <row r="31" spans="1:12" ht="17.399999999999999" customHeight="1">
+    <row r="31" spans="1:12" ht="17.45" customHeight="1">
       <c r="A31" s="13">
         <v>672000</v>
       </c>
@@ -4258,7 +4080,7 @@
         <v>Keine Aktivierung</v>
       </c>
     </row>
-    <row r="32" spans="1:12" ht="17.399999999999999" customHeight="1">
+    <row r="32" spans="1:12" ht="17.45" customHeight="1">
       <c r="A32" s="13">
         <v>671800</v>
       </c>
@@ -4311,7 +4133,7 @@
         <v>Keine Aktivierung</v>
       </c>
     </row>
-    <row r="33" spans="1:12" ht="17.399999999999999" customHeight="1">
+    <row r="33" spans="1:12" ht="17.45" customHeight="1">
       <c r="A33" s="13">
         <v>671700</v>
       </c>
@@ -4364,7 +4186,7 @@
         <v>Keine Aktivierung</v>
       </c>
     </row>
-    <row r="34" spans="1:12" ht="17.399999999999999" customHeight="1">
+    <row r="34" spans="1:12" ht="17.45" customHeight="1">
       <c r="A34" s="13">
         <v>671900</v>
       </c>
@@ -4417,7 +4239,7 @@
         <v>Keine Aktivierung</v>
       </c>
     </row>
-    <row r="35" spans="1:12" ht="17.399999999999999" customHeight="1">
+    <row r="35" spans="1:12" ht="17.45" customHeight="1">
       <c r="A35" s="13">
         <v>672100</v>
       </c>
@@ -4470,7 +4292,7 @@
         <v>Keine Aktivierung</v>
       </c>
     </row>
-    <row r="36" spans="1:12" ht="17.399999999999999" customHeight="1">
+    <row r="36" spans="1:12" ht="17.45" customHeight="1">
       <c r="A36" s="13">
         <v>672260</v>
       </c>
@@ -4523,7 +4345,7 @@
         <v>Keine Aktivierung</v>
       </c>
     </row>
-    <row r="37" spans="1:12" ht="17.399999999999999" customHeight="1">
+    <row r="37" spans="1:12" ht="17.45" customHeight="1">
       <c r="A37" s="13">
         <v>671000</v>
       </c>
@@ -4576,7 +4398,7 @@
         <v>Instandhaltung</v>
       </c>
     </row>
-    <row r="38" spans="1:12" ht="17.399999999999999" customHeight="1">
+    <row r="38" spans="1:12" ht="17.45" customHeight="1">
       <c r="A38" s="13">
         <v>671100</v>
       </c>
@@ -4629,7 +4451,7 @@
         <v>Instandhaltung</v>
       </c>
     </row>
-    <row r="39" spans="1:12" ht="17.399999999999999" customHeight="1">
+    <row r="39" spans="1:12" ht="17.45" customHeight="1">
       <c r="A39" s="13">
         <v>671200</v>
       </c>
@@ -4682,7 +4504,7 @@
         <v>Instandhaltung</v>
       </c>
     </row>
-    <row r="40" spans="1:12" ht="17.399999999999999" customHeight="1">
+    <row r="40" spans="1:12" ht="17.45" customHeight="1">
       <c r="A40" s="13">
         <v>671300</v>
       </c>
@@ -4735,7 +4557,7 @@
         <v>Instandhaltung</v>
       </c>
     </row>
-    <row r="41" spans="1:12" ht="17.399999999999999" customHeight="1">
+    <row r="41" spans="1:12" ht="17.45" customHeight="1">
       <c r="A41" s="13">
         <v>671400</v>
       </c>
@@ -4788,7 +4610,7 @@
         <v>Instandhaltung</v>
       </c>
     </row>
-    <row r="42" spans="1:12" ht="17.399999999999999" customHeight="1">
+    <row r="42" spans="1:12" ht="17.45" customHeight="1">
       <c r="A42" s="13">
         <v>671500</v>
       </c>
@@ -4841,7 +4663,7 @@
         <v>Instandhaltung</v>
       </c>
     </row>
-    <row r="43" spans="1:12" ht="17.399999999999999" customHeight="1">
+    <row r="43" spans="1:12" ht="17.45" customHeight="1">
       <c r="A43" s="13">
         <v>613350</v>
       </c>
@@ -4894,7 +4716,7 @@
         <v>Instandhaltung</v>
       </c>
     </row>
-    <row r="44" spans="1:12" ht="17.399999999999999" customHeight="1">
+    <row r="44" spans="1:12" ht="17.45" customHeight="1">
       <c r="A44" s="13">
         <v>661300</v>
       </c>
@@ -4947,7 +4769,7 @@
         <v>Keine Aktivierung</v>
       </c>
     </row>
-    <row r="45" spans="1:12" ht="17.399999999999999" customHeight="1">
+    <row r="45" spans="1:12" ht="17.45" customHeight="1">
       <c r="A45" s="13">
         <v>674300</v>
       </c>
@@ -5000,7 +4822,7 @@
         <v>Keine Aktivierung</v>
       </c>
     </row>
-    <row r="46" spans="1:12" ht="17.399999999999999" customHeight="1">
+    <row r="46" spans="1:12" ht="17.45" customHeight="1">
       <c r="A46" s="13">
         <v>605300</v>
       </c>
@@ -5053,7 +4875,7 @@
         <v>Aktivierung2</v>
       </c>
     </row>
-    <row r="47" spans="1:12" ht="17.399999999999999" customHeight="1">
+    <row r="47" spans="1:12" ht="17.45" customHeight="1">
       <c r="A47" s="13">
         <v>605300</v>
       </c>
@@ -5106,7 +4928,7 @@
         <v>Aktivierung1</v>
       </c>
     </row>
-    <row r="48" spans="1:12" ht="17.399999999999999" customHeight="1">
+    <row r="48" spans="1:12" ht="17.45" customHeight="1">
       <c r="A48" s="13">
         <v>605300</v>
       </c>
@@ -5134,7 +4956,7 @@
       </c>
       <c r="I48" s="28" t="str">
         <f>VLOOKUP(L48,'Logic ID'!$E:$G,3,0)</f>
-        <v>Amount, Usage, Null</v>
+        <v>Amount, Usage, Duration</v>
       </c>
       <c r="J48" s="13" t="s">
         <v>269</v>
@@ -5159,7 +4981,7 @@
         <v>Aktivierung3</v>
       </c>
     </row>
-    <row r="49" spans="1:12" ht="17.399999999999999" customHeight="1">
+    <row r="49" spans="1:12" ht="17.45" customHeight="1">
       <c r="A49" s="13">
         <v>673901</v>
       </c>
@@ -5293,7 +5115,7 @@
       </c>
       <c r="I51" s="28" t="str">
         <f>VLOOKUP(L51,'Logic ID'!$E:$G,3,0)</f>
-        <v>Usage, Duration, Null</v>
+        <v>Amount, Usage, Duration</v>
       </c>
       <c r="J51" s="20" t="s">
         <v>271</v>
@@ -5318,7 +5140,7 @@
         <v>WVDV2</v>
       </c>
     </row>
-    <row r="52" spans="1:12" ht="17.399999999999999" customHeight="1">
+    <row r="52" spans="1:12" ht="17.45" customHeight="1">
       <c r="A52" s="13">
         <v>613300</v>
       </c>
@@ -5371,7 +5193,7 @@
         <v>Keine Aktivierung</v>
       </c>
     </row>
-    <row r="53" spans="1:12" ht="17.399999999999999" customHeight="1">
+    <row r="53" spans="1:12" ht="17.45" customHeight="1">
       <c r="A53" s="13">
         <v>691000</v>
       </c>
@@ -5424,7 +5246,7 @@
         <v>Einkauf/Vertrieb</v>
       </c>
     </row>
-    <row r="54" spans="1:12" ht="17.399999999999999" customHeight="1">
+    <row r="54" spans="1:12" ht="17.45" customHeight="1">
       <c r="A54" s="13">
         <v>691100</v>
       </c>
@@ -5477,7 +5299,7 @@
         <v>Einkauf/Vertrieb</v>
       </c>
     </row>
-    <row r="55" spans="1:12" ht="17.399999999999999" customHeight="1">
+    <row r="55" spans="1:12" ht="17.45" customHeight="1">
       <c r="A55" s="13">
         <v>691200</v>
       </c>
@@ -5530,7 +5352,7 @@
         <v>Einkauf/Vertrieb</v>
       </c>
     </row>
-    <row r="56" spans="1:12" ht="17.399999999999999" customHeight="1">
+    <row r="56" spans="1:12" ht="17.45" customHeight="1">
       <c r="A56" s="13">
         <v>691210</v>
       </c>
@@ -5583,7 +5405,7 @@
         <v>Einkauf/Vertrieb</v>
       </c>
     </row>
-    <row r="57" spans="1:12" ht="17.399999999999999" customHeight="1">
+    <row r="57" spans="1:12" ht="17.45" customHeight="1">
       <c r="A57" s="13">
         <v>661711</v>
       </c>
@@ -5636,7 +5458,7 @@
         <v>Keine Aktivierung</v>
       </c>
     </row>
-    <row r="58" spans="1:12" ht="17.399999999999999" customHeight="1">
+    <row r="58" spans="1:12" ht="17.45" customHeight="1">
       <c r="A58" s="13">
         <v>673300</v>
       </c>
@@ -5689,7 +5511,7 @@
         <v>Keine Aktivierung</v>
       </c>
     </row>
-    <row r="59" spans="1:12" ht="17.399999999999999" customHeight="1">
+    <row r="59" spans="1:12" ht="17.45" customHeight="1">
       <c r="A59" s="13">
         <v>673500</v>
       </c>
@@ -5742,7 +5564,7 @@
         <v>WVDV1</v>
       </c>
     </row>
-    <row r="60" spans="1:12" ht="17.399999999999999" customHeight="1">
+    <row r="60" spans="1:12" ht="17.45" customHeight="1">
       <c r="A60" s="13">
         <v>673500</v>
       </c>
@@ -5770,7 +5592,7 @@
       </c>
       <c r="I60" s="28" t="str">
         <f>VLOOKUP(L60,'Logic ID'!$E:$G,3,0)</f>
-        <v>Usage, Duration, Null</v>
+        <v>Amount, Usage, Duration</v>
       </c>
       <c r="J60" s="20" t="s">
         <v>271</v>
@@ -5795,7 +5617,7 @@
         <v>WVDV2</v>
       </c>
     </row>
-    <row r="61" spans="1:12" ht="17.399999999999999" customHeight="1">
+    <row r="61" spans="1:12" ht="17.45" customHeight="1">
       <c r="A61" s="13">
         <v>673501</v>
       </c>
@@ -5848,7 +5670,7 @@
         <v>Keine Aktivierung</v>
       </c>
     </row>
-    <row r="62" spans="1:12" ht="17.399999999999999" customHeight="1">
+    <row r="62" spans="1:12" ht="17.45" customHeight="1">
       <c r="A62" s="13">
         <v>661000</v>
       </c>
@@ -5901,7 +5723,7 @@
         <v>Keine Aktivierung</v>
       </c>
     </row>
-    <row r="63" spans="1:12" ht="17.399999999999999" customHeight="1">
+    <row r="63" spans="1:12" ht="17.45" customHeight="1">
       <c r="A63" s="13">
         <v>661400</v>
       </c>
@@ -5954,7 +5776,7 @@
         <v>Keine Aktivierung</v>
       </c>
     </row>
-    <row r="64" spans="1:12" ht="17.399999999999999" customHeight="1">
+    <row r="64" spans="1:12" ht="17.45" customHeight="1">
       <c r="A64" s="13">
         <v>661500</v>
       </c>
@@ -6007,7 +5829,7 @@
         <v>Keine Aktivierung</v>
       </c>
     </row>
-    <row r="65" spans="1:12" ht="17.399999999999999" customHeight="1">
+    <row r="65" spans="1:12" ht="17.45" customHeight="1">
       <c r="A65" s="13">
         <v>671600</v>
       </c>
@@ -6060,7 +5882,7 @@
         <v>Keine Aktivierung</v>
       </c>
     </row>
-    <row r="66" spans="1:12" ht="17.399999999999999" customHeight="1">
+    <row r="66" spans="1:12" ht="17.45" customHeight="1">
       <c r="A66" s="13">
         <v>673700</v>
       </c>
@@ -6113,7 +5935,7 @@
         <v>WVDV1</v>
       </c>
     </row>
-    <row r="67" spans="1:12" ht="17.399999999999999" customHeight="1">
+    <row r="67" spans="1:12" ht="17.45" customHeight="1">
       <c r="A67" s="13">
         <v>673700</v>
       </c>
@@ -6141,7 +5963,7 @@
       </c>
       <c r="I67" s="28" t="str">
         <f>VLOOKUP(L67,'Logic ID'!$E:$G,3,0)</f>
-        <v>Usage, Duration, Null</v>
+        <v>Amount, Usage, Duration</v>
       </c>
       <c r="J67" s="20" t="s">
         <v>271</v>
@@ -6166,7 +5988,7 @@
         <v>WVDV2</v>
       </c>
     </row>
-    <row r="68" spans="1:12" ht="17.399999999999999" customHeight="1">
+    <row r="68" spans="1:12" ht="17.45" customHeight="1">
       <c r="A68" s="13">
         <v>674100</v>
       </c>
@@ -6219,7 +6041,7 @@
         <v>WVDV1</v>
       </c>
     </row>
-    <row r="69" spans="1:12" ht="17.399999999999999" customHeight="1">
+    <row r="69" spans="1:12" ht="17.45" customHeight="1">
       <c r="A69" s="13">
         <v>674100</v>
       </c>
@@ -6247,7 +6069,7 @@
       </c>
       <c r="I69" s="28" t="str">
         <f>VLOOKUP(L69,'Logic ID'!$E:$G,3,0)</f>
-        <v>Usage, Duration, Null</v>
+        <v>Amount, Usage, Duration</v>
       </c>
       <c r="J69" s="20" t="s">
         <v>271</v>
@@ -6272,7 +6094,7 @@
         <v>WVDV2</v>
       </c>
     </row>
-    <row r="70" spans="1:12" ht="17.399999999999999" customHeight="1">
+    <row r="70" spans="1:12" ht="17.45" customHeight="1">
       <c r="A70" s="13">
         <v>674600</v>
       </c>
@@ -6325,7 +6147,7 @@
         <v>Keine Aktivierung</v>
       </c>
     </row>
-    <row r="71" spans="1:12" ht="17.399999999999999" customHeight="1">
+    <row r="71" spans="1:12" ht="17.45" customHeight="1">
       <c r="A71" s="13">
         <v>605200</v>
       </c>
@@ -6378,7 +6200,7 @@
         <v>Aktivierung2</v>
       </c>
     </row>
-    <row r="72" spans="1:12" ht="17.399999999999999" customHeight="1">
+    <row r="72" spans="1:12" ht="17.45" customHeight="1">
       <c r="A72" s="13">
         <v>605200</v>
       </c>
@@ -6431,7 +6253,7 @@
         <v>Aktivierung1</v>
       </c>
     </row>
-    <row r="73" spans="1:12" ht="17.399999999999999" customHeight="1">
+    <row r="73" spans="1:12" ht="17.45" customHeight="1">
       <c r="A73" s="13">
         <v>605200</v>
       </c>
@@ -6459,7 +6281,7 @@
       </c>
       <c r="I73" s="28" t="str">
         <f>VLOOKUP(L73,'Logic ID'!$E:$G,3,0)</f>
-        <v>Amount, Usage, Null</v>
+        <v>Amount, Usage, Duration</v>
       </c>
       <c r="J73" s="20" t="s">
         <v>269</v>
@@ -6484,7 +6306,7 @@
         <v>Aktivierung3</v>
       </c>
     </row>
-    <row r="74" spans="1:12" ht="17.399999999999999" customHeight="1">
+    <row r="74" spans="1:12" ht="17.45" customHeight="1">
       <c r="A74" s="13">
         <v>681200</v>
       </c>
@@ -6537,7 +6359,7 @@
         <v>WVDV1</v>
       </c>
     </row>
-    <row r="75" spans="1:12" ht="17.399999999999999" customHeight="1">
+    <row r="75" spans="1:12" ht="17.45" customHeight="1">
       <c r="A75" s="13">
         <v>681200</v>
       </c>
@@ -6565,7 +6387,7 @@
       </c>
       <c r="I75" s="28" t="str">
         <f>VLOOKUP(L75,'Logic ID'!$E:$G,3,0)</f>
-        <v>Usage, Duration, Null</v>
+        <v>Amount, Usage, Duration</v>
       </c>
       <c r="J75" s="20" t="s">
         <v>271</v>
@@ -6590,7 +6412,7 @@
         <v>WVDV2</v>
       </c>
     </row>
-    <row r="76" spans="1:12" ht="17.399999999999999" customHeight="1">
+    <row r="76" spans="1:12" ht="17.45" customHeight="1">
       <c r="A76" s="13">
         <v>603400</v>
       </c>
@@ -6643,7 +6465,7 @@
         <v>Aktivierung2</v>
       </c>
     </row>
-    <row r="77" spans="1:12" ht="17.399999999999999" customHeight="1">
+    <row r="77" spans="1:12" ht="17.45" customHeight="1">
       <c r="A77" s="13">
         <v>603400</v>
       </c>
@@ -6696,7 +6518,7 @@
         <v>Aktivierung1</v>
       </c>
     </row>
-    <row r="78" spans="1:12" ht="17.399999999999999" customHeight="1">
+    <row r="78" spans="1:12" ht="17.45" customHeight="1">
       <c r="A78" s="13">
         <v>603400</v>
       </c>
@@ -6724,7 +6546,7 @@
       </c>
       <c r="I78" s="28" t="str">
         <f>VLOOKUP(L78,'Logic ID'!$E:$G,3,0)</f>
-        <v>Amount, Usage, Null</v>
+        <v>Amount, Usage, Duration</v>
       </c>
       <c r="J78" s="20" t="s">
         <v>269</v>
@@ -6749,7 +6571,7 @@
         <v>Aktivierung3</v>
       </c>
     </row>
-    <row r="79" spans="1:12" ht="17.399999999999999" customHeight="1">
+    <row r="79" spans="1:12" ht="17.45" customHeight="1">
       <c r="A79" s="13">
         <v>605210</v>
       </c>
@@ -6802,7 +6624,7 @@
         <v>Aktivierung2</v>
       </c>
     </row>
-    <row r="80" spans="1:12" ht="17.399999999999999" customHeight="1">
+    <row r="80" spans="1:12" ht="17.45" customHeight="1">
       <c r="A80" s="13">
         <v>605210</v>
       </c>
@@ -6855,7 +6677,7 @@
         <v>Aktivierung1</v>
       </c>
     </row>
-    <row r="81" spans="1:12" ht="17.399999999999999" customHeight="1">
+    <row r="81" spans="1:12" ht="17.45" customHeight="1">
       <c r="A81" s="13">
         <v>605210</v>
       </c>
@@ -6883,7 +6705,7 @@
       </c>
       <c r="I81" s="28" t="str">
         <f>VLOOKUP(L81,'Logic ID'!$E:$G,3,0)</f>
-        <v>Amount, Usage, Null</v>
+        <v>Amount, Usage, Duration</v>
       </c>
       <c r="J81" s="20" t="s">
         <v>269</v>
@@ -6908,7 +6730,7 @@
         <v>Aktivierung3</v>
       </c>
     </row>
-    <row r="82" spans="1:12" ht="17.399999999999999" customHeight="1">
+    <row r="82" spans="1:12" ht="17.45" customHeight="1">
       <c r="A82" s="13">
         <v>673200</v>
       </c>
@@ -6961,7 +6783,7 @@
         <v>Keine Aktivierung</v>
       </c>
     </row>
-    <row r="83" spans="1:12" ht="17.399999999999999" customHeight="1">
+    <row r="83" spans="1:12" ht="17.45" customHeight="1">
       <c r="A83" s="13">
         <v>673400</v>
       </c>
@@ -7014,7 +6836,7 @@
         <v>Keine Aktivierung</v>
       </c>
     </row>
-    <row r="84" spans="1:12" ht="17.399999999999999" customHeight="1">
+    <row r="84" spans="1:12" ht="17.45" customHeight="1">
       <c r="A84" s="13">
         <v>695300</v>
       </c>
@@ -7067,7 +6889,7 @@
         <v>Keine Aktivierung</v>
       </c>
     </row>
-    <row r="85" spans="1:12" ht="17.399999999999999" customHeight="1">
+    <row r="85" spans="1:12" ht="17.45" customHeight="1">
       <c r="A85" s="13">
         <v>695400</v>
       </c>
@@ -7120,7 +6942,7 @@
         <v>Aktivierung2</v>
       </c>
     </row>
-    <row r="86" spans="1:12" ht="17.399999999999999" customHeight="1">
+    <row r="86" spans="1:12" ht="17.45" customHeight="1">
       <c r="A86" s="13">
         <v>695400</v>
       </c>
@@ -7173,7 +6995,7 @@
         <v>Aktivierung1</v>
       </c>
     </row>
-    <row r="87" spans="1:12" ht="17.399999999999999" customHeight="1">
+    <row r="87" spans="1:12" ht="17.45" customHeight="1">
       <c r="A87" s="13">
         <v>695400</v>
       </c>
@@ -7201,7 +7023,7 @@
       </c>
       <c r="I87" s="28" t="str">
         <f>VLOOKUP(L87,'Logic ID'!$E:$G,3,0)</f>
-        <v>Amount, Usage, Null</v>
+        <v>Amount, Usage, Duration</v>
       </c>
       <c r="J87" s="20" t="s">
         <v>269</v>
@@ -7226,7 +7048,7 @@
         <v>Aktivierung3</v>
       </c>
     </row>
-    <row r="88" spans="1:12" ht="17.399999999999999" customHeight="1">
+    <row r="88" spans="1:12" ht="17.45" customHeight="1">
       <c r="A88" s="13">
         <v>605100</v>
       </c>
@@ -7279,7 +7101,7 @@
         <v>Aktivierung2</v>
       </c>
     </row>
-    <row r="89" spans="1:12" ht="17.399999999999999" customHeight="1">
+    <row r="89" spans="1:12" ht="17.45" customHeight="1">
       <c r="A89" s="13">
         <v>605100</v>
       </c>
@@ -7332,7 +7154,7 @@
         <v>Aktivierung1</v>
       </c>
     </row>
-    <row r="90" spans="1:12" ht="17.399999999999999" customHeight="1">
+    <row r="90" spans="1:12" ht="17.45" customHeight="1">
       <c r="A90" s="13">
         <v>605100</v>
       </c>
@@ -7360,7 +7182,7 @@
       </c>
       <c r="I90" s="28" t="str">
         <f>VLOOKUP(L90,'Logic ID'!$E:$G,3,0)</f>
-        <v>Amount, Usage, Null</v>
+        <v>Amount, Usage, Duration</v>
       </c>
       <c r="J90" s="20" t="s">
         <v>269</v>
@@ -7385,7 +7207,7 @@
         <v>Aktivierung3</v>
       </c>
     </row>
-    <row r="91" spans="1:12" ht="17.399999999999999" customHeight="1">
+    <row r="91" spans="1:12" ht="17.45" customHeight="1">
       <c r="A91" s="13">
         <v>674400</v>
       </c>
@@ -7438,7 +7260,7 @@
         <v>WVDV1</v>
       </c>
     </row>
-    <row r="92" spans="1:12" ht="17.399999999999999" customHeight="1">
+    <row r="92" spans="1:12" ht="17.45" customHeight="1">
       <c r="A92" s="13">
         <v>674400</v>
       </c>
@@ -7466,7 +7288,7 @@
       </c>
       <c r="I92" s="28" t="str">
         <f>VLOOKUP(L92,'Logic ID'!$E:$G,3,0)</f>
-        <v>Usage, Duration, Null</v>
+        <v>Amount, Usage, Duration</v>
       </c>
       <c r="J92" s="13" t="s">
         <v>271</v>
@@ -7491,7 +7313,7 @@
         <v>WVDV2</v>
       </c>
     </row>
-    <row r="93" spans="1:12" ht="17.399999999999999" customHeight="1">
+    <row r="93" spans="1:12" ht="17.45" customHeight="1">
       <c r="A93" s="13">
         <v>607700</v>
       </c>
@@ -7544,7 +7366,7 @@
         <v>Keine Aktivierung</v>
       </c>
     </row>
-    <row r="94" spans="1:12" ht="17.399999999999999" customHeight="1">
+    <row r="94" spans="1:12" ht="17.45" customHeight="1">
       <c r="A94" s="13">
         <v>608030</v>
       </c>
@@ -7597,7 +7419,7 @@
         <v>Keine Aktivierung</v>
       </c>
     </row>
-    <row r="95" spans="1:12" ht="17.399999999999999" customHeight="1">
+    <row r="95" spans="1:12" ht="17.45" customHeight="1">
       <c r="A95" s="13">
         <v>605400</v>
       </c>
@@ -7650,7 +7472,7 @@
         <v>Keine Aktivierung</v>
       </c>
     </row>
-    <row r="96" spans="1:12" ht="17.399999999999999" customHeight="1">
+    <row r="96" spans="1:12" ht="17.45" customHeight="1">
       <c r="A96" s="13">
         <v>694900</v>
       </c>
@@ -7703,7 +7525,7 @@
         <v>Keine Aktivierung</v>
       </c>
     </row>
-    <row r="97" spans="1:12" ht="17.399999999999999" customHeight="1">
+    <row r="97" spans="1:12" ht="17.45" customHeight="1">
       <c r="A97" s="13">
         <v>695000</v>
       </c>
@@ -7756,7 +7578,7 @@
         <v>Keine Aktivierung</v>
       </c>
     </row>
-    <row r="98" spans="1:12" ht="17.399999999999999" customHeight="1">
+    <row r="98" spans="1:12" ht="17.45" customHeight="1">
       <c r="A98" s="13">
         <v>695100</v>
       </c>
@@ -7809,7 +7631,7 @@
         <v>Keine Aktivierung</v>
       </c>
     </row>
-    <row r="99" spans="1:12" ht="17.399999999999999" customHeight="1">
+    <row r="99" spans="1:12" ht="17.45" customHeight="1">
       <c r="A99" s="13">
         <v>695200</v>
       </c>
@@ -7862,7 +7684,7 @@
         <v>Keine Aktivierung</v>
       </c>
     </row>
-    <row r="100" spans="1:12" ht="17.399999999999999" customHeight="1">
+    <row r="100" spans="1:12" ht="17.45" customHeight="1">
       <c r="A100" s="13">
         <v>673600</v>
       </c>
@@ -7915,7 +7737,7 @@
         <v>Keine Aktivierung</v>
       </c>
     </row>
-    <row r="101" spans="1:12" ht="17.399999999999999" customHeight="1">
+    <row r="101" spans="1:12" ht="17.45" customHeight="1">
       <c r="A101" s="13">
         <v>662400</v>
       </c>
@@ -7968,7 +7790,7 @@
         <v>Keine Aktivierung</v>
       </c>
     </row>
-    <row r="102" spans="1:12" ht="17.399999999999999" customHeight="1">
+    <row r="102" spans="1:12" ht="17.45" customHeight="1">
       <c r="A102" s="13">
         <v>662500</v>
       </c>
@@ -8021,7 +7843,7 @@
         <v>Keine Aktivierung</v>
       </c>
     </row>
-    <row r="103" spans="1:12" ht="17.399999999999999" customHeight="1">
+    <row r="103" spans="1:12" ht="17.45" customHeight="1">
       <c r="A103" s="13">
         <v>672310</v>
       </c>
@@ -8074,7 +7896,7 @@
         <v>Keine Aktivierung</v>
       </c>
     </row>
-    <row r="104" spans="1:12" ht="17.399999999999999" customHeight="1">
+    <row r="104" spans="1:12" ht="17.45" customHeight="1">
       <c r="A104" s="13">
         <v>672320</v>
       </c>
@@ -8127,7 +7949,7 @@
         <v>Keine Aktivierung</v>
       </c>
     </row>
-    <row r="105" spans="1:12" ht="17.399999999999999" customHeight="1">
+    <row r="105" spans="1:12" ht="17.45" customHeight="1">
       <c r="A105" s="13">
         <v>672400</v>
       </c>
@@ -8180,7 +8002,7 @@
         <v>Keine Aktivierung</v>
       </c>
     </row>
-    <row r="106" spans="1:12" ht="17.399999999999999" customHeight="1">
+    <row r="106" spans="1:12" ht="17.45" customHeight="1">
       <c r="A106" s="13">
         <v>672500</v>
       </c>
@@ -8233,7 +8055,7 @@
         <v>Keine Aktivierung</v>
       </c>
     </row>
-    <row r="107" spans="1:12" ht="17.399999999999999" customHeight="1">
+    <row r="107" spans="1:12" ht="17.45" customHeight="1">
       <c r="A107" s="13">
         <v>672600</v>
       </c>
@@ -8286,7 +8108,7 @@
         <v>Keine Aktivierung</v>
       </c>
     </row>
-    <row r="108" spans="1:12" ht="17.399999999999999" customHeight="1">
+    <row r="108" spans="1:12" ht="17.45" customHeight="1">
       <c r="A108" s="13">
         <v>672700</v>
       </c>
@@ -8339,7 +8161,7 @@
         <v>Keine Aktivierung</v>
       </c>
     </row>
-    <row r="109" spans="1:12" ht="17.399999999999999" customHeight="1">
+    <row r="109" spans="1:12" ht="17.45" customHeight="1">
       <c r="A109" s="13">
         <v>604400</v>
       </c>
@@ -8392,7 +8214,7 @@
         <v>Einkauf/Vertrieb</v>
       </c>
     </row>
-    <row r="110" spans="1:12" ht="17.399999999999999" customHeight="1">
+    <row r="110" spans="1:12" ht="17.45" customHeight="1">
       <c r="A110" s="13">
         <v>604300</v>
       </c>
@@ -8445,7 +8267,7 @@
         <v>Einkauf/Vertrieb</v>
       </c>
     </row>
-    <row r="111" spans="1:12" ht="17.399999999999999" customHeight="1">
+    <row r="111" spans="1:12" ht="17.45" customHeight="1">
       <c r="A111" s="13">
         <v>604310</v>
       </c>
@@ -8498,7 +8320,7 @@
         <v>Einkauf/Vertrieb</v>
       </c>
     </row>
-    <row r="112" spans="1:12" ht="17.399999999999999" customHeight="1">
+    <row r="112" spans="1:12" ht="17.45" customHeight="1">
       <c r="A112" s="13">
         <v>604000</v>
       </c>
@@ -8551,7 +8373,7 @@
         <v>Einkauf/Vertrieb</v>
       </c>
     </row>
-    <row r="113" spans="1:12" ht="17.399999999999999" customHeight="1">
+    <row r="113" spans="1:12" ht="17.45" customHeight="1">
       <c r="A113" s="13">
         <v>691300</v>
       </c>
@@ -8604,7 +8426,7 @@
         <v>Einkauf/Vertrieb</v>
       </c>
     </row>
-    <row r="114" spans="1:12" ht="17.399999999999999" customHeight="1">
+    <row r="114" spans="1:12" ht="17.45" customHeight="1">
       <c r="A114" s="13">
         <v>691310</v>
       </c>
@@ -8657,7 +8479,7 @@
         <v>Einkauf/Vertrieb</v>
       </c>
     </row>
-    <row r="115" spans="1:12" ht="17.399999999999999" customHeight="1">
+    <row r="115" spans="1:12" ht="17.45" customHeight="1">
       <c r="A115" s="13">
         <v>691350</v>
       </c>
@@ -8710,7 +8532,7 @@
         <v>Einkauf/Vertrieb</v>
       </c>
     </row>
-    <row r="116" spans="1:12" ht="17.399999999999999" customHeight="1">
+    <row r="116" spans="1:12" ht="17.45" customHeight="1">
       <c r="A116" s="13">
         <v>661150</v>
       </c>
@@ -8763,7 +8585,7 @@
         <v>Keine Aktivierung</v>
       </c>
     </row>
-    <row r="117" spans="1:12" ht="17.399999999999999" customHeight="1">
+    <row r="117" spans="1:12" ht="17.45" customHeight="1">
       <c r="A117" s="13">
         <v>999910</v>
       </c>
@@ -8819,7 +8641,7 @@
   </sheetData>
   <autoFilter ref="A1:L117" xr:uid="{A2546393-D3F3-4891-9180-301BCA80D3AD}"/>
   <conditionalFormatting sqref="L1:L1048576">
-    <cfRule type="cellIs" dxfId="26" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="29" operator="equal">
       <formula>"missing"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8839,14 +8661,14 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.45" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="5" customWidth="1"/>
-    <col min="2" max="2" width="10.33203125" style="5" customWidth="1"/>
-    <col min="3" max="256" width="8.88671875" style="5" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" style="5" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" style="5" customWidth="1"/>
+    <col min="3" max="256" width="8.85546875" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:256" ht="14.4" customHeight="1">
+    <row r="1" spans="1:256" ht="14.45" customHeight="1">
       <c r="A1" s="10" t="s">
         <v>249</v>
       </c>
@@ -9108,7 +8930,7 @@
       <c r="IU1" s="10"/>
       <c r="IV1" s="10"/>
     </row>
-    <row r="2" spans="1:256" ht="14.4" customHeight="1">
+    <row r="2" spans="1:256" ht="14.45" customHeight="1">
       <c r="A2" s="2">
         <v>0</v>
       </c>
@@ -9133,7 +8955,7 @@
       <c r="R2" s="4"/>
       <c r="S2" s="4"/>
     </row>
-    <row r="3" spans="1:256" ht="14.4" customHeight="1">
+    <row r="3" spans="1:256" ht="14.45" customHeight="1">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -9158,7 +8980,7 @@
       <c r="R3" s="4"/>
       <c r="S3" s="4"/>
     </row>
-    <row r="4" spans="1:256" ht="14.4" customHeight="1">
+    <row r="4" spans="1:256" ht="14.45" customHeight="1">
       <c r="A4" s="2">
         <v>2</v>
       </c>
@@ -9183,7 +9005,7 @@
       <c r="R4" s="4"/>
       <c r="S4" s="4"/>
     </row>
-    <row r="5" spans="1:256" ht="14.4" customHeight="1">
+    <row r="5" spans="1:256" ht="14.45" customHeight="1">
       <c r="A5" s="2">
         <v>3</v>
       </c>
@@ -9208,7 +9030,7 @@
       <c r="R5" s="4"/>
       <c r="S5" s="4"/>
     </row>
-    <row r="6" spans="1:256" ht="14.4" customHeight="1">
+    <row r="6" spans="1:256" ht="14.45" customHeight="1">
       <c r="A6" s="2">
         <v>4</v>
       </c>
@@ -9233,7 +9055,7 @@
       <c r="R6" s="4"/>
       <c r="S6" s="4"/>
     </row>
-    <row r="7" spans="1:256" ht="14.4" customHeight="1">
+    <row r="7" spans="1:256" ht="14.45" customHeight="1">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -9254,7 +9076,7 @@
       <c r="R7" s="4"/>
       <c r="S7" s="4"/>
     </row>
-    <row r="8" spans="1:256" ht="14.4" customHeight="1">
+    <row r="8" spans="1:256" ht="14.45" customHeight="1">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -9275,7 +9097,7 @@
       <c r="R8" s="4"/>
       <c r="S8" s="4"/>
     </row>
-    <row r="9" spans="1:256" ht="14.4" customHeight="1">
+    <row r="9" spans="1:256" ht="14.45" customHeight="1">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -9296,7 +9118,7 @@
       <c r="R9" s="4"/>
       <c r="S9" s="4"/>
     </row>
-    <row r="10" spans="1:256" ht="14.4" customHeight="1">
+    <row r="10" spans="1:256" ht="14.45" customHeight="1">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -9317,7 +9139,7 @@
       <c r="R10" s="4"/>
       <c r="S10" s="4"/>
     </row>
-    <row r="11" spans="1:256" ht="14.4" customHeight="1">
+    <row r="11" spans="1:256" ht="14.45" customHeight="1">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -9338,7 +9160,7 @@
       <c r="R11" s="4"/>
       <c r="S11" s="4"/>
     </row>
-    <row r="12" spans="1:256" ht="14.4" customHeight="1">
+    <row r="12" spans="1:256" ht="14.45" customHeight="1">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
@@ -9377,12 +9199,12 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.45" customHeight="1"/>
   <cols>
-    <col min="1" max="256" width="8.88671875" style="6" customWidth="1"/>
+    <col min="1" max="256" width="8.85546875" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:256" ht="14.4" customHeight="1">
+    <row r="1" spans="1:256" ht="14.45" customHeight="1">
       <c r="A1" s="10" t="s">
         <v>249</v>
       </c>
@@ -9644,7 +9466,7 @@
       <c r="IU1" s="10"/>
       <c r="IV1" s="10"/>
     </row>
-    <row r="2" spans="1:256" ht="14.4" customHeight="1">
+    <row r="2" spans="1:256" ht="14.45" customHeight="1">
       <c r="A2" s="2">
         <v>0</v>
       </c>
@@ -9667,7 +9489,7 @@
       <c r="P2" s="4"/>
       <c r="Q2" s="4"/>
     </row>
-    <row r="3" spans="1:256" ht="14.4" customHeight="1">
+    <row r="3" spans="1:256" ht="14.45" customHeight="1">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -9690,7 +9512,7 @@
       <c r="P3" s="4"/>
       <c r="Q3" s="4"/>
     </row>
-    <row r="4" spans="1:256" ht="14.4" customHeight="1">
+    <row r="4" spans="1:256" ht="14.45" customHeight="1">
       <c r="A4" s="2">
         <v>2</v>
       </c>
@@ -9713,7 +9535,7 @@
       <c r="P4" s="4"/>
       <c r="Q4" s="4"/>
     </row>
-    <row r="5" spans="1:256" ht="14.4" customHeight="1">
+    <row r="5" spans="1:256" ht="14.45" customHeight="1">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -9732,7 +9554,7 @@
       <c r="P5" s="4"/>
       <c r="Q5" s="4"/>
     </row>
-    <row r="6" spans="1:256" ht="14.4" customHeight="1">
+    <row r="6" spans="1:256" ht="14.45" customHeight="1">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -9751,7 +9573,7 @@
       <c r="P6" s="4"/>
       <c r="Q6" s="4"/>
     </row>
-    <row r="7" spans="1:256" ht="14.4" customHeight="1">
+    <row r="7" spans="1:256" ht="14.45" customHeight="1">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -9770,7 +9592,7 @@
       <c r="P7" s="4"/>
       <c r="Q7" s="4"/>
     </row>
-    <row r="8" spans="1:256" ht="14.4" customHeight="1">
+    <row r="8" spans="1:256" ht="14.45" customHeight="1">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -9789,7 +9611,7 @@
       <c r="P8" s="4"/>
       <c r="Q8" s="4"/>
     </row>
-    <row r="9" spans="1:256" ht="14.4" customHeight="1">
+    <row r="9" spans="1:256" ht="14.45" customHeight="1">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -9808,7 +9630,7 @@
       <c r="P9" s="4"/>
       <c r="Q9" s="4"/>
     </row>
-    <row r="10" spans="1:256" ht="14.4" customHeight="1">
+    <row r="10" spans="1:256" ht="14.45" customHeight="1">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -9827,7 +9649,7 @@
       <c r="P10" s="4"/>
       <c r="Q10" s="4"/>
     </row>
-    <row r="11" spans="1:256" ht="14.4" customHeight="1">
+    <row r="11" spans="1:256" ht="14.45" customHeight="1">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -9858,17 +9680,17 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:IS91"/>
+  <dimension ref="A1:IQ91"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.45" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="7" customWidth="1"/>
-    <col min="2" max="2" width="127.88671875" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="253" width="8.88671875" style="7" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" style="7" customWidth="1"/>
+    <col min="2" max="2" width="127.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="251" width="8.85546875" style="7" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15" customHeight="1">
@@ -9879,7 +9701,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="17.399999999999999" customHeight="1">
+    <row r="2" spans="1:2" ht="17.45" customHeight="1">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -9887,7 +9709,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="17.399999999999999" customHeight="1">
+    <row r="3" spans="1:2" ht="17.45" customHeight="1">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -9895,7 +9717,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="17.399999999999999" customHeight="1">
+    <row r="4" spans="1:2" ht="17.45" customHeight="1">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -9903,7 +9725,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="17.399999999999999" customHeight="1">
+    <row r="5" spans="1:2" ht="17.45" customHeight="1">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -9911,7 +9733,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="17.399999999999999" customHeight="1">
+    <row r="6" spans="1:2" ht="17.45" customHeight="1">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -9919,7 +9741,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="17.399999999999999" customHeight="1">
+    <row r="7" spans="1:2" ht="17.45" customHeight="1">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -9927,7 +9749,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="17.399999999999999" customHeight="1">
+    <row r="8" spans="1:2" ht="17.45" customHeight="1">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -9935,7 +9757,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="17.399999999999999" customHeight="1">
+    <row r="9" spans="1:2" ht="17.45" customHeight="1">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -9943,7 +9765,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="17.399999999999999" customHeight="1">
+    <row r="10" spans="1:2" ht="17.45" customHeight="1">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -9951,7 +9773,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="17.399999999999999" customHeight="1">
+    <row r="11" spans="1:2" ht="17.45" customHeight="1">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -9959,7 +9781,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="17.399999999999999" customHeight="1">
+    <row r="12" spans="1:2" ht="17.45" customHeight="1">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -9967,7 +9789,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="17.399999999999999" customHeight="1">
+    <row r="13" spans="1:2" ht="17.45" customHeight="1">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -9975,7 +9797,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="17.399999999999999" customHeight="1">
+    <row r="14" spans="1:2" ht="17.45" customHeight="1">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -9983,7 +9805,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="17.399999999999999" customHeight="1">
+    <row r="15" spans="1:2" ht="17.45" customHeight="1">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -9991,7 +9813,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="17.399999999999999" customHeight="1">
+    <row r="16" spans="1:2" ht="17.45" customHeight="1">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -9999,7 +9821,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="17.399999999999999" customHeight="1">
+    <row r="17" spans="1:2" ht="17.45" customHeight="1">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -10007,7 +9829,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="17.399999999999999" customHeight="1">
+    <row r="18" spans="1:2" ht="17.45" customHeight="1">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -10015,7 +9837,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="17.399999999999999" customHeight="1">
+    <row r="19" spans="1:2" ht="17.45" customHeight="1">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -10023,7 +9845,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="17.399999999999999" customHeight="1">
+    <row r="20" spans="1:2" ht="17.45" customHeight="1">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -10031,7 +9853,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="17.399999999999999" customHeight="1">
+    <row r="21" spans="1:2" ht="17.45" customHeight="1">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -10039,7 +9861,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="17.399999999999999" customHeight="1">
+    <row r="22" spans="1:2" ht="17.45" customHeight="1">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -10047,7 +9869,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="17.399999999999999" customHeight="1">
+    <row r="23" spans="1:2" ht="17.45" customHeight="1">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -10055,7 +9877,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="17.399999999999999" customHeight="1">
+    <row r="24" spans="1:2" ht="17.45" customHeight="1">
       <c r="A24" s="2">
         <v>23</v>
       </c>
@@ -10063,7 +9885,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="17.399999999999999" customHeight="1">
+    <row r="25" spans="1:2" ht="17.45" customHeight="1">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -10071,7 +9893,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="17.399999999999999" customHeight="1">
+    <row r="26" spans="1:2" ht="17.45" customHeight="1">
       <c r="A26" s="2">
         <v>25</v>
       </c>
@@ -10079,7 +9901,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="17.399999999999999" customHeight="1">
+    <row r="27" spans="1:2" ht="17.45" customHeight="1">
       <c r="A27" s="2">
         <v>26</v>
       </c>
@@ -10087,7 +9909,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="17.399999999999999" customHeight="1">
+    <row r="28" spans="1:2" ht="17.45" customHeight="1">
       <c r="A28" s="2">
         <v>27</v>
       </c>
@@ -10095,7 +9917,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="17.399999999999999" customHeight="1">
+    <row r="29" spans="1:2" ht="17.45" customHeight="1">
       <c r="A29" s="2">
         <v>28</v>
       </c>
@@ -10103,7 +9925,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="17.399999999999999" customHeight="1">
+    <row r="30" spans="1:2" ht="17.45" customHeight="1">
       <c r="A30" s="2">
         <v>29</v>
       </c>
@@ -10111,7 +9933,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="17.399999999999999" customHeight="1">
+    <row r="31" spans="1:2" ht="17.45" customHeight="1">
       <c r="A31" s="2">
         <v>30</v>
       </c>
@@ -10119,7 +9941,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="17.399999999999999" customHeight="1">
+    <row r="32" spans="1:2" ht="17.45" customHeight="1">
       <c r="A32" s="2">
         <v>31</v>
       </c>
@@ -10127,7 +9949,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="17.399999999999999" customHeight="1">
+    <row r="33" spans="1:2" ht="17.45" customHeight="1">
       <c r="A33" s="2">
         <v>32</v>
       </c>
@@ -10135,7 +9957,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="17.399999999999999" customHeight="1">
+    <row r="34" spans="1:2" ht="17.45" customHeight="1">
       <c r="A34" s="2">
         <v>33</v>
       </c>
@@ -10143,7 +9965,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="17.399999999999999" customHeight="1">
+    <row r="35" spans="1:2" ht="17.45" customHeight="1">
       <c r="A35" s="2">
         <v>34</v>
       </c>
@@ -10151,7 +9973,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="17.399999999999999" customHeight="1">
+    <row r="36" spans="1:2" ht="17.45" customHeight="1">
       <c r="A36" s="2">
         <v>35</v>
       </c>
@@ -10159,7 +9981,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="17.399999999999999" customHeight="1">
+    <row r="37" spans="1:2" ht="17.45" customHeight="1">
       <c r="A37" s="2">
         <v>36</v>
       </c>
@@ -10167,7 +9989,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="17.399999999999999" customHeight="1">
+    <row r="38" spans="1:2" ht="17.45" customHeight="1">
       <c r="A38" s="2">
         <v>37</v>
       </c>
@@ -10175,7 +9997,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="17.399999999999999" customHeight="1">
+    <row r="39" spans="1:2" ht="17.45" customHeight="1">
       <c r="A39" s="2">
         <v>38</v>
       </c>
@@ -10191,7 +10013,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="17.399999999999999" customHeight="1">
+    <row r="41" spans="1:2" ht="17.45" customHeight="1">
       <c r="A41" s="2">
         <v>40</v>
       </c>
@@ -10199,7 +10021,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="17.399999999999999" customHeight="1">
+    <row r="42" spans="1:2" ht="17.45" customHeight="1">
       <c r="A42" s="2">
         <v>41</v>
       </c>
@@ -10207,7 +10029,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="43" spans="1:2" ht="17.399999999999999" customHeight="1">
+    <row r="43" spans="1:2" ht="17.45" customHeight="1">
       <c r="A43" s="2">
         <v>42</v>
       </c>
@@ -10215,7 +10037,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="17.399999999999999" customHeight="1">
+    <row r="44" spans="1:2" ht="17.45" customHeight="1">
       <c r="A44" s="2">
         <v>43</v>
       </c>
@@ -10223,7 +10045,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="45" spans="1:2" ht="17.399999999999999" customHeight="1">
+    <row r="45" spans="1:2" ht="17.45" customHeight="1">
       <c r="A45" s="2">
         <v>44</v>
       </c>
@@ -10231,7 +10053,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="46" spans="1:2" ht="17.399999999999999" customHeight="1">
+    <row r="46" spans="1:2" ht="17.45" customHeight="1">
       <c r="A46" s="2">
         <v>45</v>
       </c>
@@ -10239,7 +10061,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="47" spans="1:2" ht="17.399999999999999" customHeight="1">
+    <row r="47" spans="1:2" ht="17.45" customHeight="1">
       <c r="A47" s="2">
         <v>46</v>
       </c>
@@ -10247,7 +10069,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="48" spans="1:2" ht="17.399999999999999" customHeight="1">
+    <row r="48" spans="1:2" ht="17.45" customHeight="1">
       <c r="A48" s="2">
         <v>47</v>
       </c>
@@ -10255,7 +10077,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="17.399999999999999" customHeight="1">
+    <row r="49" spans="1:2" ht="17.45" customHeight="1">
       <c r="A49" s="2">
         <v>48</v>
       </c>
@@ -10263,7 +10085,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="50" spans="1:2" ht="17.399999999999999" customHeight="1">
+    <row r="50" spans="1:2" ht="17.45" customHeight="1">
       <c r="A50" s="2">
         <v>49</v>
       </c>
@@ -10271,7 +10093,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="51" spans="1:2" ht="17.399999999999999" customHeight="1">
+    <row r="51" spans="1:2" ht="17.45" customHeight="1">
       <c r="A51" s="2">
         <v>50</v>
       </c>
@@ -10279,7 +10101,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="52" spans="1:2" ht="17.399999999999999" customHeight="1">
+    <row r="52" spans="1:2" ht="17.45" customHeight="1">
       <c r="A52" s="2">
         <v>51</v>
       </c>
@@ -10287,7 +10109,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="53" spans="1:2" ht="17.399999999999999" customHeight="1">
+    <row r="53" spans="1:2" ht="17.45" customHeight="1">
       <c r="A53" s="2">
         <v>52</v>
       </c>
@@ -10295,7 +10117,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="54" spans="1:2" ht="17.399999999999999" customHeight="1">
+    <row r="54" spans="1:2" ht="17.45" customHeight="1">
       <c r="A54" s="2">
         <v>53</v>
       </c>
@@ -10303,7 +10125,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="55" spans="1:2" ht="17.399999999999999" customHeight="1">
+    <row r="55" spans="1:2" ht="17.45" customHeight="1">
       <c r="A55" s="2">
         <v>54</v>
       </c>
@@ -10311,7 +10133,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="56" spans="1:2" ht="17.399999999999999" customHeight="1">
+    <row r="56" spans="1:2" ht="17.45" customHeight="1">
       <c r="A56" s="2">
         <v>55</v>
       </c>
@@ -10319,7 +10141,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="57" spans="1:2" ht="17.399999999999999" customHeight="1">
+    <row r="57" spans="1:2" ht="17.45" customHeight="1">
       <c r="A57" s="2">
         <v>56</v>
       </c>
@@ -10327,7 +10149,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="58" spans="1:2" ht="17.399999999999999" customHeight="1">
+    <row r="58" spans="1:2" ht="17.45" customHeight="1">
       <c r="A58" s="2">
         <v>57</v>
       </c>
@@ -10335,7 +10157,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="59" spans="1:2" ht="17.399999999999999" customHeight="1">
+    <row r="59" spans="1:2" ht="17.45" customHeight="1">
       <c r="A59" s="2">
         <v>58</v>
       </c>
@@ -10343,7 +10165,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="60" spans="1:2" ht="17.399999999999999" customHeight="1">
+    <row r="60" spans="1:2" ht="17.45" customHeight="1">
       <c r="A60" s="2">
         <v>59</v>
       </c>
@@ -10351,7 +10173,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="61" spans="1:2" ht="17.399999999999999" customHeight="1">
+    <row r="61" spans="1:2" ht="17.45" customHeight="1">
       <c r="A61" s="2">
         <v>60</v>
       </c>
@@ -10359,7 +10181,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="62" spans="1:2" ht="17.399999999999999" customHeight="1">
+    <row r="62" spans="1:2" ht="17.45" customHeight="1">
       <c r="A62" s="2">
         <v>61</v>
       </c>
@@ -10367,7 +10189,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="63" spans="1:2" ht="17.399999999999999" customHeight="1">
+    <row r="63" spans="1:2" ht="17.45" customHeight="1">
       <c r="A63" s="2">
         <v>62</v>
       </c>
@@ -10375,7 +10197,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="64" spans="1:2" ht="17.399999999999999" customHeight="1">
+    <row r="64" spans="1:2" ht="17.45" customHeight="1">
       <c r="A64" s="2">
         <v>63</v>
       </c>
@@ -10383,7 +10205,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="65" spans="1:2" ht="17.399999999999999" customHeight="1">
+    <row r="65" spans="1:2" ht="17.45" customHeight="1">
       <c r="A65" s="2">
         <v>64</v>
       </c>
@@ -10391,7 +10213,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="66" spans="1:2" ht="17.399999999999999" customHeight="1">
+    <row r="66" spans="1:2" ht="17.45" customHeight="1">
       <c r="A66" s="2">
         <v>65</v>
       </c>
@@ -10399,7 +10221,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="67" spans="1:2" ht="17.399999999999999" customHeight="1">
+    <row r="67" spans="1:2" ht="17.45" customHeight="1">
       <c r="A67" s="2">
         <v>66</v>
       </c>
@@ -10407,7 +10229,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="68" spans="1:2" ht="17.399999999999999" customHeight="1">
+    <row r="68" spans="1:2" ht="17.45" customHeight="1">
       <c r="A68" s="2">
         <v>67</v>
       </c>
@@ -10415,7 +10237,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="69" spans="1:2" ht="17.399999999999999" customHeight="1">
+    <row r="69" spans="1:2" ht="17.45" customHeight="1">
       <c r="A69" s="2">
         <v>68</v>
       </c>
@@ -10423,7 +10245,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="70" spans="1:2" ht="17.399999999999999" customHeight="1">
+    <row r="70" spans="1:2" ht="17.45" customHeight="1">
       <c r="A70" s="2">
         <v>69</v>
       </c>
@@ -10431,7 +10253,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="71" spans="1:2" ht="17.399999999999999" customHeight="1">
+    <row r="71" spans="1:2" ht="17.45" customHeight="1">
       <c r="A71" s="2">
         <v>70</v>
       </c>
@@ -10439,7 +10261,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="72" spans="1:2" ht="17.399999999999999" customHeight="1">
+    <row r="72" spans="1:2" ht="17.45" customHeight="1">
       <c r="A72" s="2">
         <v>71</v>
       </c>
@@ -10447,7 +10269,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="73" spans="1:2" ht="17.399999999999999" customHeight="1">
+    <row r="73" spans="1:2" ht="17.45" customHeight="1">
       <c r="A73" s="2">
         <v>72</v>
       </c>
@@ -10455,7 +10277,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="74" spans="1:2" ht="17.399999999999999" customHeight="1">
+    <row r="74" spans="1:2" ht="17.45" customHeight="1">
       <c r="A74" s="2">
         <v>73</v>
       </c>
@@ -10463,7 +10285,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="75" spans="1:2" ht="17.399999999999999" customHeight="1">
+    <row r="75" spans="1:2" ht="17.45" customHeight="1">
       <c r="A75" s="2">
         <v>74</v>
       </c>
@@ -10471,7 +10293,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="76" spans="1:2" ht="17.399999999999999" customHeight="1">
+    <row r="76" spans="1:2" ht="17.45" customHeight="1">
       <c r="A76" s="2">
         <v>75</v>
       </c>
@@ -10479,7 +10301,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="77" spans="1:2" ht="17.399999999999999" customHeight="1">
+    <row r="77" spans="1:2" ht="17.45" customHeight="1">
       <c r="A77" s="2">
         <v>76</v>
       </c>
@@ -10487,7 +10309,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="78" spans="1:2" ht="17.399999999999999" customHeight="1">
+    <row r="78" spans="1:2" ht="17.45" customHeight="1">
       <c r="A78" s="2">
         <v>77</v>
       </c>
@@ -10495,7 +10317,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="79" spans="1:2" ht="17.399999999999999" customHeight="1">
+    <row r="79" spans="1:2" ht="17.45" customHeight="1">
       <c r="A79" s="2">
         <v>78</v>
       </c>
@@ -10503,7 +10325,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="80" spans="1:2" ht="17.399999999999999" customHeight="1">
+    <row r="80" spans="1:2" ht="17.45" customHeight="1">
       <c r="A80" s="2">
         <v>79</v>
       </c>
@@ -10511,7 +10333,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="81" spans="1:2" ht="17.399999999999999" customHeight="1">
+    <row r="81" spans="1:2" ht="17.45" customHeight="1">
       <c r="A81" s="2">
         <v>80</v>
       </c>
@@ -10519,7 +10341,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="82" spans="1:2" ht="17.399999999999999" customHeight="1">
+    <row r="82" spans="1:2" ht="17.45" customHeight="1">
       <c r="A82" s="2">
         <v>81</v>
       </c>
@@ -10527,7 +10349,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="83" spans="1:2" ht="17.399999999999999" customHeight="1">
+    <row r="83" spans="1:2" ht="17.45" customHeight="1">
       <c r="A83" s="2">
         <v>82</v>
       </c>
@@ -10535,7 +10357,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="84" spans="1:2" ht="17.399999999999999" customHeight="1">
+    <row r="84" spans="1:2" ht="17.45" customHeight="1">
       <c r="A84" s="2">
         <v>83</v>
       </c>
@@ -10543,7 +10365,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="85" spans="1:2" ht="17.399999999999999" customHeight="1">
+    <row r="85" spans="1:2" ht="17.45" customHeight="1">
       <c r="A85" s="2">
         <v>84</v>
       </c>
@@ -10551,7 +10373,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="86" spans="1:2" ht="17.399999999999999" customHeight="1">
+    <row r="86" spans="1:2" ht="17.45" customHeight="1">
       <c r="A86" s="2">
         <v>85</v>
       </c>
@@ -10559,7 +10381,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="87" spans="1:2" ht="17.399999999999999" customHeight="1">
+    <row r="87" spans="1:2" ht="17.45" customHeight="1">
       <c r="A87" s="2">
         <v>86</v>
       </c>
@@ -10567,7 +10389,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="88" spans="1:2" ht="17.399999999999999" customHeight="1">
+    <row r="88" spans="1:2" ht="17.45" customHeight="1">
       <c r="A88" s="2">
         <v>87</v>
       </c>
@@ -10575,7 +10397,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="89" spans="1:2" ht="17.399999999999999" customHeight="1">
+    <row r="89" spans="1:2" ht="17.45" customHeight="1">
       <c r="A89" s="2">
         <v>88</v>
       </c>
@@ -10583,7 +10405,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="90" spans="1:2" ht="17.399999999999999" customHeight="1">
+    <row r="90" spans="1:2" ht="17.45" customHeight="1">
       <c r="A90" s="2">
         <v>89</v>
       </c>
@@ -10591,7 +10413,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="91" spans="1:2" ht="17.399999999999999" customHeight="1">
+    <row r="91" spans="1:2" ht="17.45" customHeight="1">
       <c r="A91" s="2">
         <v>90</v>
       </c>
@@ -10616,9 +10438,9 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -10679,25 +10501,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:IW24"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.45" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="3.5546875" style="8" customWidth="1"/>
-    <col min="2" max="2" width="16.5546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.88671875" style="8" customWidth="1"/>
-    <col min="4" max="4" width="8.88671875" style="8" customWidth="1"/>
-    <col min="5" max="5" width="18.6640625" style="10" customWidth="1"/>
-    <col min="6" max="6" width="32.6640625" style="8" customWidth="1"/>
-    <col min="7" max="7" width="32.6640625" style="10" customWidth="1"/>
-    <col min="8" max="21" width="8.88671875" style="8" customWidth="1"/>
-    <col min="22" max="22" width="22.6640625" style="8" customWidth="1"/>
-    <col min="23" max="257" width="8.88671875" style="8" customWidth="1"/>
+    <col min="1" max="1" width="3.5703125" style="8" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" style="8" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" style="8" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" style="10" customWidth="1"/>
+    <col min="6" max="6" width="32.7109375" style="8" customWidth="1"/>
+    <col min="7" max="7" width="32.7109375" style="10" customWidth="1"/>
+    <col min="8" max="21" width="8.85546875" style="8" customWidth="1"/>
+    <col min="22" max="22" width="22.7109375" style="8" customWidth="1"/>
+    <col min="23" max="257" width="8.85546875" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:257" ht="14.4" customHeight="1">
+    <row r="1" spans="1:257" ht="14.45" customHeight="1">
       <c r="A1" s="4"/>
       <c r="B1" s="4"/>
       <c r="C1" s="31" t="s">
@@ -10731,7 +10553,7 @@
       <c r="U1" s="4"/>
       <c r="V1" s="4"/>
     </row>
-    <row r="2" spans="1:257" ht="14.4" customHeight="1">
+    <row r="2" spans="1:257" ht="14.45" customHeight="1">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -10769,7 +10591,7 @@
       <c r="U2" s="4"/>
       <c r="V2" s="4"/>
     </row>
-    <row r="3" spans="1:257" ht="14.4" customHeight="1">
+    <row r="3" spans="1:257" ht="14.45" customHeight="1">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -10807,7 +10629,7 @@
       <c r="U3" s="4"/>
       <c r="V3" s="4"/>
     </row>
-    <row r="4" spans="1:257" ht="14.4" customHeight="1">
+    <row r="4" spans="1:257" ht="14.45" customHeight="1">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -10845,7 +10667,7 @@
       <c r="U4" s="4"/>
       <c r="V4" s="4"/>
     </row>
-    <row r="5" spans="1:257" ht="14.4" customHeight="1">
+    <row r="5" spans="1:257" ht="14.45" customHeight="1">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -10864,8 +10686,8 @@
       <c r="F5" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="G5" s="1" t="s">
-        <v>281</v>
+      <c r="G5" s="32" t="s">
+        <v>288</v>
       </c>
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
@@ -10883,7 +10705,7 @@
       <c r="U5" s="4"/>
       <c r="V5" s="4"/>
     </row>
-    <row r="6" spans="1:257" ht="14.4" customHeight="1">
+    <row r="6" spans="1:257" ht="14.45" customHeight="1">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -10921,7 +10743,7 @@
       <c r="U6" s="4"/>
       <c r="V6"/>
     </row>
-    <row r="7" spans="1:257" ht="14.4" customHeight="1">
+    <row r="7" spans="1:257" ht="14.45" customHeight="1">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -10959,7 +10781,7 @@
       <c r="U7" s="4"/>
       <c r="V7" s="4"/>
     </row>
-    <row r="8" spans="1:257" ht="14.4" customHeight="1">
+    <row r="8" spans="1:257" ht="14.45" customHeight="1">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -10978,8 +10800,8 @@
       <c r="F8" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G8" s="1" t="s">
-        <v>289</v>
+      <c r="G8" s="32" t="s">
+        <v>288</v>
       </c>
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
@@ -10997,7 +10819,7 @@
       <c r="U8" s="4"/>
       <c r="V8"/>
     </row>
-    <row r="9" spans="1:257" ht="14.4" customHeight="1">
+    <row r="9" spans="1:257" ht="14.45" customHeight="1">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -11035,7 +10857,7 @@
       <c r="U9" s="4"/>
       <c r="V9"/>
     </row>
-    <row r="10" spans="1:257" ht="14.4" customHeight="1">
+    <row r="10" spans="1:257" ht="14.45" customHeight="1">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -11073,7 +10895,7 @@
       <c r="U10" s="4"/>
       <c r="V10" s="4"/>
     </row>
-    <row r="11" spans="1:257" ht="14.4" customHeight="1">
+    <row r="11" spans="1:257" ht="14.45" customHeight="1">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -11111,7 +10933,7 @@
       <c r="U11" s="4"/>
       <c r="V11" s="4"/>
     </row>
-    <row r="12" spans="1:257" ht="14.4" customHeight="1">
+    <row r="12" spans="1:257" ht="14.45" customHeight="1">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -11149,7 +10971,7 @@
       <c r="U12" s="4"/>
       <c r="V12" s="4"/>
     </row>
-    <row r="13" spans="1:257" ht="14.4" customHeight="1">
+    <row r="13" spans="1:257" ht="14.45" customHeight="1">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -11187,7 +11009,7 @@
       <c r="U13" s="4"/>
       <c r="V13" s="4"/>
     </row>
-    <row r="14" spans="1:257" ht="14.4" customHeight="1">
+    <row r="14" spans="1:257" ht="14.45" customHeight="1">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -11225,7 +11047,7 @@
       <c r="U14" s="4"/>
       <c r="V14"/>
     </row>
-    <row r="15" spans="1:257" ht="14.4" customHeight="1">
+    <row r="15" spans="1:257" ht="14.45" customHeight="1">
       <c r="A15" s="2"/>
       <c r="B15" s="1"/>
       <c r="C15" s="2"/>
@@ -11484,7 +11306,7 @@
       <c r="IV15" s="10"/>
       <c r="IW15" s="10"/>
     </row>
-    <row r="16" spans="1:257" ht="14.4" customHeight="1">
+    <row r="16" spans="1:257" ht="14.45" customHeight="1">
       <c r="A16" s="2"/>
       <c r="B16" s="1"/>
       <c r="C16" s="2"/>
@@ -11743,7 +11565,7 @@
       <c r="IV16" s="10"/>
       <c r="IW16" s="10"/>
     </row>
-    <row r="17" spans="1:257" ht="14.4" customHeight="1">
+    <row r="17" spans="1:257" ht="14.45" customHeight="1">
       <c r="A17" s="2"/>
       <c r="B17" s="1"/>
       <c r="C17" s="2"/>
@@ -12002,7 +11824,7 @@
       <c r="IV17" s="10"/>
       <c r="IW17" s="10"/>
     </row>
-    <row r="18" spans="1:257" ht="14.4" customHeight="1">
+    <row r="18" spans="1:257" ht="14.45" customHeight="1">
       <c r="A18" s="2"/>
       <c r="B18" s="1"/>
       <c r="C18" s="2"/>
@@ -12261,7 +12083,7 @@
       <c r="IV18" s="10"/>
       <c r="IW18" s="10"/>
     </row>
-    <row r="19" spans="1:257" ht="14.4" customHeight="1">
+    <row r="19" spans="1:257" ht="14.45" customHeight="1">
       <c r="A19" s="2"/>
       <c r="B19" s="1"/>
       <c r="C19" s="2"/>
@@ -12520,7 +12342,7 @@
       <c r="IV19" s="10"/>
       <c r="IW19" s="10"/>
     </row>
-    <row r="20" spans="1:257" ht="14.4" customHeight="1">
+    <row r="20" spans="1:257" ht="14.45" customHeight="1">
       <c r="A20" s="2"/>
       <c r="B20" s="1"/>
       <c r="C20" s="2"/>
@@ -12779,7 +12601,7 @@
       <c r="IV20" s="10"/>
       <c r="IW20" s="10"/>
     </row>
-    <row r="21" spans="1:257" ht="14.4" customHeight="1">
+    <row r="21" spans="1:257" ht="14.45" customHeight="1">
       <c r="A21" s="2"/>
       <c r="B21" s="1"/>
       <c r="C21" s="2"/>
@@ -13038,7 +12860,7 @@
       <c r="IV21" s="10"/>
       <c r="IW21" s="10"/>
     </row>
-    <row r="22" spans="1:257" ht="14.4" customHeight="1">
+    <row r="22" spans="1:257" ht="14.45" customHeight="1">
       <c r="A22" s="2"/>
       <c r="B22" s="1"/>
       <c r="C22" s="2"/>
@@ -13297,7 +13119,7 @@
       <c r="IV22" s="10"/>
       <c r="IW22" s="10"/>
     </row>
-    <row r="23" spans="1:257" ht="14.4" customHeight="1">
+    <row r="23" spans="1:257" ht="14.45" customHeight="1">
       <c r="A23" s="2"/>
       <c r="B23" s="1"/>
       <c r="C23" s="2"/>
@@ -13556,7 +13378,7 @@
       <c r="IV23" s="10"/>
       <c r="IW23" s="10"/>
     </row>
-    <row r="24" spans="1:257" ht="14.4" customHeight="1">
+    <row r="24" spans="1:257" ht="14.45" customHeight="1">
       <c r="A24" s="2"/>
       <c r="B24" s="1"/>
       <c r="C24" s="2"/>
@@ -13826,6 +13648,54 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxKeywordTaxHTField xmlns="45be70f0-66b9-4629-a389-4b080fc0dfa6">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">t55170</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">2a7bebd1-4a65-4a83-8880-9af9f7738c6c</TermId>
+        </TermInfo>
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">HP SAP S4 ACCOUNT IDENTIFIER FEJLESZTES NP</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">2711dfa3-6ec1-413d-8823-997cd6be3ca9</TermId>
+        </TermInfo>
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">CO＆FI_S/4 HANA Concept</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">bfc7b42e-ea39-4d21-8ccd-32d67d914123</TermId>
+        </TermInfo>
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">O＆O_Procurement</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">68c352b4-4d41-43f2-b180-79522b747923</TermId>
+        </TermInfo>
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">CO＆FI_Accounting</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">df76b3e5-5a8d-4c97-a933-1c42bdf53c62</TermId>
+        </TermInfo>
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Intercompany</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">4467356c-29d0-45c7-bb32-7599fd4b7437</TermId>
+        </TermInfo>
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">p_30003</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">530d64dc-cb80-49da-a923-511a942d9ac0</TermId>
+        </TermInfo>
+      </Terms>
+    </TaxKeywordTaxHTField>
+    <TaxCatchAll xmlns="45be70f0-66b9-4629-a389-4b080fc0dfa6">
+      <Value>7</Value>
+      <Value>6</Value>
+      <Value>5</Value>
+      <Value>4</Value>
+      <Value>3</Value>
+      <Value>2</Value>
+      <Value>1</Value>
+    </TaxCatchAll>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokumentum" ma:contentTypeID="0x0101008B0F08FECF9ACD44B69B0979475AA3A3" ma:contentTypeVersion="5" ma:contentTypeDescription="Új dokumentum létrehozása." ma:contentTypeScope="" ma:versionID="15e7cafbdefa31d60e781c5e4062628f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="45be70f0-66b9-4629-a389-4b080fc0dfa6" xmlns:ns3="cc54d3cb-87fe-4b6a-be2e-e1fd0be84e77" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f81e6785b8b81ecd23d6e742c299b13f" ns2:_="" ns3:_="">
     <xsd:import namespace="45be70f0-66b9-4629-a389-4b080fc0dfa6"/>
@@ -13982,54 +13852,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxKeywordTaxHTField xmlns="45be70f0-66b9-4629-a389-4b080fc0dfa6">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">t55170</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">2a7bebd1-4a65-4a83-8880-9af9f7738c6c</TermId>
-        </TermInfo>
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">HP SAP S4 ACCOUNT IDENTIFIER FEJLESZTES NP</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">2711dfa3-6ec1-413d-8823-997cd6be3ca9</TermId>
-        </TermInfo>
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">CO＆FI_S/4 HANA Concept</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">bfc7b42e-ea39-4d21-8ccd-32d67d914123</TermId>
-        </TermInfo>
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">O＆O_Procurement</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">68c352b4-4d41-43f2-b180-79522b747923</TermId>
-        </TermInfo>
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">CO＆FI_Accounting</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">df76b3e5-5a8d-4c97-a933-1c42bdf53c62</TermId>
-        </TermInfo>
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Intercompany</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">4467356c-29d0-45c7-bb32-7599fd4b7437</TermId>
-        </TermInfo>
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">p_30003</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">530d64dc-cb80-49da-a923-511a942d9ac0</TermId>
-        </TermInfo>
-      </Terms>
-    </TaxKeywordTaxHTField>
-    <TaxCatchAll xmlns="45be70f0-66b9-4629-a389-4b080fc0dfa6">
-      <Value>7</Value>
-      <Value>6</Value>
-      <Value>5</Value>
-      <Value>4</Value>
-      <Value>3</Value>
-      <Value>2</Value>
-      <Value>1</Value>
-    </TaxCatchAll>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -14040,6 +13862,16 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4141748-E8CF-4376-BEDF-0CE4C9A34F7B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="45be70f0-66b9-4629-a389-4b080fc0dfa6"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{47BF3E90-0828-4759-ACA7-3670C46D50E8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -14058,16 +13890,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4141748-E8CF-4376-BEDF-0CE4C9A34F7B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="45be70f0-66b9-4629-a389-4b080fc0dfa6"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DC021B46-1420-4ED7-AC55-8BF0CD9341B9}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
"" bug, new keywords
</commit_message>
<xml_diff>
--- a/Datei.xlsx
+++ b/Datei.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cts\Documents\SEA\sea\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51506270-AEA0-4A19-AD57-1AD5595B78A8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9E15E489-75ED-4293-BA19-DE5471D20FF1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="789" uniqueCount="362">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="789" uniqueCount="363">
   <si>
     <t>Account ID</t>
   </si>
@@ -187,9 +187,6 @@
     <t>KPMG,PwC,Deloitte,Ernst,Young,EY,Big4,Beratung,Coach</t>
   </si>
   <si>
-    <t>Beratungskosten "Big4" (KPMG, PwC, Deloitte, EY)</t>
-  </si>
-  <si>
     <t>Seminarkosten</t>
   </si>
   <si>
@@ -682,6 +679,9 @@
     <t>Geschenk3</t>
   </si>
   <si>
+    <t>Amount, Usage, Duration</t>
+  </si>
+  <si>
     <t>c6</t>
   </si>
   <si>
@@ -730,18 +730,6 @@
     <t>Einkauf, Vertrieb</t>
   </si>
   <si>
-    <t>Tasche,Geschenk,Kugelschreiber,Anhänger,Beutel,Armbanduhr,USB,Buch,Tasse,Becher,Blume,schenken,Armband</t>
-  </si>
-  <si>
-    <t>Armbanduhr,USB,Kugelschreiber,Shirt,Geschenk,Hemd,Modell,Schirm,Quizaktion,Schuhe,schenken,Box,Hose,Hotel,Gutschein,Poster,Becher,Tasche</t>
-  </si>
-  <si>
-    <t>Polo,Karten,Kugelschreiber,Geburtstag,Verpflegung,Blume,Schokolade,Geschenk,Armbanduhr,USB,Team,Abendessen,Messe,Modellauto,Bewirtung,Gutschein,Tasse,Becher,schenken</t>
-  </si>
-  <si>
-    <t>Ausbildung,Schulung,Seminar,Training,Kurs,Weiterbildung,Workshop,Geschenk,Modellauto,Bewirtung,Sicherheit,Gutschein,Tasse,Becher,Tasche,Poster,Bild,Polo,schenken</t>
-  </si>
-  <si>
     <t>Stick,Schutz,Schuhe,Jacke,T-Shirt,Helm,Größe,Bluse,Hemd,Socke,Name,Herr,Frau,Mitarbeiter,Betrieb,Produktion,Dame,Beruf,Sicherheit</t>
   </si>
   <si>
@@ -769,9 +757,6 @@
     <t>Seminar,Kosten,Schulung,Inhouse,Kurs,Gebühr,Training,Anmeldung,Gefahrgut,Webinar</t>
   </si>
   <si>
-    <t>Mieteen,Server,Computer,EDV,Rampe,Medien,Technik,Zaun,Müllbehälter,Drucker,Anlage,Maschine,Nutzfahrzeuge,Kältekammer,Möbel,Telefon,Container,Sport</t>
-  </si>
-  <si>
     <t>Entsendung,Umzug,Kurs,Steuerberatungskosten,Caregroupkosten,Versicherung,Übersetzung,Kultur,Mieteen,Haushalt,Arbeitszimmer</t>
   </si>
   <si>
@@ -1087,9 +1072,6 @@
     <t>Geschenk,Hotel,Mieten,Bahn,Instandhaltung,Reparatur,Ersatzteil,Ersetzen,Entwicklung,Flug</t>
   </si>
   <si>
-    <t>Aufsichtsrat,Instandhaltung,Reparatur,Ersatzteil,Ersetzen,Entwicklung,Mieten</t>
-  </si>
-  <si>
     <t>Geschenk,Hotel,Mieten,Instandhaltung,Reparatur,Ersatzteil,Ersetzen,Entwicklung,Flug</t>
   </si>
   <si>
@@ -1111,26 +1093,47 @@
     <t>Modell</t>
   </si>
   <si>
-    <t>Ausgangsfracht,Wartung,Instandhaltung,Leasing,Beratung,Reinigung,Geschenk,Bewirtung,Hotel,Mieten,Frühstück,Mitarbeiter,Catering,Seminar</t>
-  </si>
-  <si>
-    <t>Ausgangsfracht,Wartung,Instandhaltung,Leasing,Beratung,Reinigung,Geschenk,Bewirtung,Hotel,Mieten,Frühstück,Mitarbeiter,Catering,Seminar,Ersatzteil</t>
-  </si>
-  <si>
-    <t>Ausgangsfracht,Wartung,Instandhaltung,Leasing,Beratung,Reinigung,Geschenk,Bewirtung,Hotel,Mieten,Frühstück,Mitarbeiter,Catering,Seminar,Lieferant</t>
-  </si>
-  <si>
-    <t>Ausgangsfracht,Wartung,Instandhaltung,Leasing,Beratung,Reinigung,Geschenk,Bewirtung,Hotel,Mieten,Frühstück,Mitarbeiter,Catering,Seminar,Qualität</t>
-  </si>
-  <si>
-    <t>Amount, Duration, Usage</t>
+    <t>Mieten,Server,Computer,EDV,Rampe,Medien,Technik,Zaun,Müllbehälter,Drucker,Anlage,Maschine,Nutzfahrzeuge,Kältekammer,Möbel,Telefon,Container,Sport</t>
+  </si>
+  <si>
+    <t>Tasche,Geschenk,Kugelschreiber,Anhänger,Beutel,Armbanduhr,USB,Buch,Tasse,Becher,Blume,schenken,Armband,Kalender</t>
+  </si>
+  <si>
+    <t>Armbanduhr,USB,Kugelschreiber,Shirt,Geschenk,Hemd,Modell,Schirm,Quizaktion,Schuhe,schenken,Box,Hose,Hotel,Gutschein,Poster,Becher,Tasche,Kalender</t>
+  </si>
+  <si>
+    <t>Polo,Karten,Kugelschreiber,Geburtstag,Verpflegung,Blume,Schokolade,Geschenk,Armbanduhr,USB,Team,Abendessen,Messe,Modellauto,Bewirtung,Gutschein,Tasse,Becher,schenken,Kalender</t>
+  </si>
+  <si>
+    <t>Ausbildung,Schulung,Seminar,Training,Kurs,Weiterbildung,Workshop,Geschenk,Modellauto,Bewirtung,Sicherheit,Gutschein,Tasse,Becher,Tasche,Poster,Bild,Polo,schenken,Kalender</t>
+  </si>
+  <si>
+    <t>Ausgangsfracht,Wartung,Instandhaltung,Leasing,Beratung,Reinigung,Geschenk,Bewirtung,Hotel,Mieten,Frühstück,Mitarbeiter,Catering,Seminar,Reparatur</t>
+  </si>
+  <si>
+    <t>Ausgangsfracht,Wartung,Instandhaltung,Leasing,Beratung,Reinigung,Geschenk,Bewirtung,Hotel,Mieten,Frühstück,Mitarbeiter,Catering,Seminar,Ersatzteil,Reparatur</t>
+  </si>
+  <si>
+    <t>Ausgangsfracht,Wartung,Instandhaltung,Leasing,Beratung,Reinigung,Geschenk,Bewirtung,Hotel,Mieten,Frühstück,Mitarbeiter,Catering,Seminar,Lieferant,Reparatur</t>
+  </si>
+  <si>
+    <t>Ausgangsfracht,Wartung,Instandhaltung,Leasing,Beratung,Reinigung,Geschenk,Bewirtung,Hotel,Mieten,Frühstück,Mitarbeiter,Catering,Seminar,Qualität,Reparatur</t>
+  </si>
+  <si>
+    <t>Mieten,Reparatur,Ersatzteil,Ersetzen,Entwicklung,Instandhaltung,Wartung</t>
+  </si>
+  <si>
+    <t>Aufsichtsrat,Instandhaltung,Reparatur,Ersatzteil,Ersetzen,Entwicklung,Mieten,Wartung</t>
+  </si>
+  <si>
+    <t>Beratungskosten Big4 (KPMG, PwC, Deloitte, EY)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -1173,13 +1176,6 @@
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="238"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1326,10 +1322,10 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
@@ -2662,11 +2658,11 @@
   <sheetPr codeName="Munka1"/>
   <dimension ref="A1:L117"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D20" sqref="D20"/>
+      <selection pane="bottomRight" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.45" customHeight="1"/>
@@ -2696,31 +2692,31 @@
         <v>2</v>
       </c>
       <c r="D1" s="29" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E1" s="14" t="s">
         <v>3</v>
       </c>
       <c r="F1" s="15" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="G1" s="29" t="s">
         <v>4</v>
       </c>
       <c r="H1" s="15" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="I1" s="15" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="J1" s="29" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="K1" s="15" t="s">
         <v>5</v>
       </c>
       <c r="L1" s="15" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="17.45" customHeight="1">
@@ -2731,10 +2727,10 @@
         <v>6</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>230</v>
+        <v>352</v>
       </c>
       <c r="D2" s="28" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="E2" s="16">
         <v>1</v>
@@ -2754,7 +2750,7 @@
         <v>Amount, Usage, Null</v>
       </c>
       <c r="J2" s="13" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="K2" s="11" t="s">
         <v>8</v>
@@ -2784,10 +2780,10 @@
         <v>9</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>231</v>
+        <v>353</v>
       </c>
       <c r="D3" s="28" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="E3" s="19">
         <v>0</v>
@@ -2807,7 +2803,7 @@
         <v>Usage, Null, Null</v>
       </c>
       <c r="J3" s="20" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="K3" s="12" t="s">
         <v>8</v>
@@ -2837,10 +2833,10 @@
         <v>11</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>232</v>
+        <v>354</v>
       </c>
       <c r="D4" s="28" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="E4" s="21">
         <v>1.2</v>
@@ -2860,7 +2856,7 @@
         <v>Amount, Usage, Null</v>
       </c>
       <c r="J4" s="20" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="K4" s="11" t="s">
         <v>8</v>
@@ -2890,10 +2886,10 @@
         <v>13</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>233</v>
+        <v>355</v>
       </c>
       <c r="D5" s="28" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="E5" s="21">
         <v>3.4</v>
@@ -2913,7 +2909,7 @@
         <v>Amount, Usage, Null</v>
       </c>
       <c r="J5" s="20" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="K5" s="11" t="s">
         <v>8</v>
@@ -2943,10 +2939,10 @@
         <v>15</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="D6" s="28" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="E6" s="17">
         <v>4</v>
@@ -2963,10 +2959,10 @@
       </c>
       <c r="I6" s="28" t="str">
         <f>VLOOKUP(L6,'Logic ID'!$E:$G,3,0)</f>
-        <v>Amount, Duration, Usage</v>
+        <v>Amount, Usage, Duration</v>
       </c>
       <c r="J6" s="20" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="K6" s="12" t="s">
         <v>17</v>
@@ -2996,10 +2992,10 @@
         <v>15</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="D7" s="28" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="E7" s="17">
         <v>4</v>
@@ -3016,10 +3012,10 @@
       </c>
       <c r="I7" s="28" t="str">
         <f>VLOOKUP(L7,'Logic ID'!$E:$G,3,0)</f>
-        <v>Amount, Duration, Usage</v>
+        <v>Amount, Usage, Duration</v>
       </c>
       <c r="J7" s="20" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="K7" s="12" t="s">
         <v>17</v>
@@ -3049,13 +3045,13 @@
         <v>15</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="D8" s="28" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="E8" s="21" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F8" s="17">
         <v>0</v>
@@ -3069,10 +3065,10 @@
       </c>
       <c r="I8" s="28" t="str">
         <f>VLOOKUP(L8,'Logic ID'!$E:$G,3,0)</f>
-        <v>Amount, Duration, Usage</v>
+        <v>Amount, Usage, Duration</v>
       </c>
       <c r="J8" s="20" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="K8" s="12" t="s">
         <v>17</v>
@@ -3102,10 +3098,10 @@
         <v>18</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="D9" s="28" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="E9" s="17">
         <v>4</v>
@@ -3122,10 +3118,10 @@
       </c>
       <c r="I9" s="28" t="str">
         <f>VLOOKUP(L9,'Logic ID'!$E:$G,3,0)</f>
-        <v>Amount, Duration, Usage</v>
+        <v>Amount, Usage, Duration</v>
       </c>
       <c r="J9" s="20" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="K9" s="12" t="s">
         <v>17</v>
@@ -3155,10 +3151,10 @@
         <v>18</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="D10" s="28" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="E10" s="17">
         <v>4</v>
@@ -3175,10 +3171,10 @@
       </c>
       <c r="I10" s="28" t="str">
         <f>VLOOKUP(L10,'Logic ID'!$E:$G,3,0)</f>
-        <v>Amount, Duration, Usage</v>
+        <v>Amount, Usage, Duration</v>
       </c>
       <c r="J10" s="20" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="K10" s="12" t="s">
         <v>17</v>
@@ -3208,13 +3204,13 @@
         <v>18</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="D11" s="28" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="E11" s="21" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F11" s="17">
         <v>0</v>
@@ -3228,10 +3224,10 @@
       </c>
       <c r="I11" s="28" t="str">
         <f>VLOOKUP(L11,'Logic ID'!$E:$G,3,0)</f>
-        <v>Amount, Duration, Usage</v>
+        <v>Amount, Usage, Duration</v>
       </c>
       <c r="J11" s="20" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="K11" s="12" t="s">
         <v>17</v>
@@ -3261,10 +3257,10 @@
         <v>20</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="D12" s="28" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="E12" s="17">
         <v>4</v>
@@ -3281,10 +3277,10 @@
       </c>
       <c r="I12" s="28" t="str">
         <f>VLOOKUP(L12,'Logic ID'!$E:$G,3,0)</f>
-        <v>Amount, Duration, Usage</v>
+        <v>Amount, Usage, Duration</v>
       </c>
       <c r="J12" s="20" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="K12" s="12" t="s">
         <v>17</v>
@@ -3314,10 +3310,10 @@
         <v>20</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="D13" s="28" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="E13" s="17">
         <v>4</v>
@@ -3334,10 +3330,10 @@
       </c>
       <c r="I13" s="28" t="str">
         <f>VLOOKUP(L13,'Logic ID'!$E:$G,3,0)</f>
-        <v>Amount, Duration, Usage</v>
+        <v>Amount, Usage, Duration</v>
       </c>
       <c r="J13" s="20" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="K13" s="12" t="s">
         <v>17</v>
@@ -3367,13 +3363,13 @@
         <v>20</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="D14" s="28" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="E14" s="21" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F14" s="17">
         <v>0</v>
@@ -3387,10 +3383,10 @@
       </c>
       <c r="I14" s="28" t="str">
         <f>VLOOKUP(L14,'Logic ID'!$E:$G,3,0)</f>
-        <v>Amount, Duration, Usage</v>
+        <v>Amount, Usage, Duration</v>
       </c>
       <c r="J14" s="20" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="K14" s="12" t="s">
         <v>17</v>
@@ -3420,10 +3416,10 @@
         <v>22</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="D15" s="28" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="E15" s="19">
         <v>0</v>
@@ -3443,7 +3439,7 @@
         <v>Usage, Null, Null</v>
       </c>
       <c r="J15" s="13" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="K15" s="12" t="s">
         <v>8</v>
@@ -3473,10 +3469,10 @@
         <v>24</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>243</v>
+        <v>351</v>
       </c>
       <c r="D16" s="28" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="E16" s="21">
         <v>0</v>
@@ -3526,10 +3522,10 @@
         <v>27</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="D17" s="28" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="E17" s="21">
         <v>0</v>
@@ -3579,10 +3575,10 @@
         <v>29</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="D18" s="28" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="E18" s="21">
         <v>0</v>
@@ -3635,7 +3631,7 @@
         <v>32</v>
       </c>
       <c r="D19" s="28" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="E19" s="21">
         <v>0</v>
@@ -3688,7 +3684,7 @@
         <v>35</v>
       </c>
       <c r="D20" s="28" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="E20" s="21">
         <v>0</v>
@@ -3738,10 +3734,10 @@
         <v>37</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="D21" s="28" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="E21" s="21">
         <v>0</v>
@@ -3794,7 +3790,7 @@
         <v>40</v>
       </c>
       <c r="D22" s="28" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="E22" s="21">
         <v>0</v>
@@ -3844,10 +3840,10 @@
         <v>42</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="D23" s="28" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="E23" s="21">
         <v>0</v>
@@ -3897,10 +3893,10 @@
         <v>44</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="D24" s="28" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="E24" s="17">
         <v>4</v>
@@ -3917,10 +3913,10 @@
       </c>
       <c r="I24" s="28" t="str">
         <f>VLOOKUP(L24,'Logic ID'!$E:$G,3,0)</f>
-        <v>Amount, Duration, Usage</v>
+        <v>Amount, Usage, Duration</v>
       </c>
       <c r="J24" s="20" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K24" s="12" t="s">
         <v>46</v>
@@ -3950,10 +3946,10 @@
         <v>44</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="D25" s="28" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="E25" s="17">
         <v>0</v>
@@ -3970,10 +3966,10 @@
       </c>
       <c r="I25" s="28" t="str">
         <f>VLOOKUP(L25,'Logic ID'!$E:$G,3,0)</f>
-        <v>Amount, Duration, Usage</v>
+        <v>Amount, Usage, Duration</v>
       </c>
       <c r="J25" s="20" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K25" s="12" t="s">
         <v>46</v>
@@ -4005,8 +4001,8 @@
       <c r="C26" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="D26" s="32" t="s">
-        <v>301</v>
+      <c r="D26" s="33" t="s">
+        <v>296</v>
       </c>
       <c r="E26" s="17">
         <v>4</v>
@@ -4023,10 +4019,10 @@
       </c>
       <c r="I26" s="28" t="str">
         <f>VLOOKUP(L26,'Logic ID'!$E:$G,3,0)</f>
-        <v>Amount, Duration, Usage</v>
+        <v>Amount, Usage, Duration</v>
       </c>
       <c r="J26" s="20" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K26" s="12" t="s">
         <v>46</v>
@@ -4058,8 +4054,8 @@
       <c r="C27" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="D27" s="32" t="s">
-        <v>301</v>
+      <c r="D27" s="33" t="s">
+        <v>296</v>
       </c>
       <c r="E27" s="17">
         <v>0</v>
@@ -4076,10 +4072,10 @@
       </c>
       <c r="I27" s="28" t="str">
         <f>VLOOKUP(L27,'Logic ID'!$E:$G,3,0)</f>
-        <v>Amount, Duration, Usage</v>
+        <v>Amount, Usage, Duration</v>
       </c>
       <c r="J27" s="20" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K27" s="12" t="s">
         <v>46</v>
@@ -4106,13 +4102,13 @@
         <v>661200</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="D28" s="28" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="E28" s="21">
         <v>0</v>
@@ -4159,13 +4155,13 @@
         <v>681153</v>
       </c>
       <c r="B29" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="C29" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="C29" s="12" t="s">
-        <v>52</v>
-      </c>
       <c r="D29" s="28" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="E29" s="21">
         <v>0</v>
@@ -4212,13 +4208,13 @@
         <v>672201</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="D30" s="28" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="E30" s="21">
         <v>0</v>
@@ -4265,13 +4261,13 @@
         <v>672000</v>
       </c>
       <c r="B31" s="12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="D31" s="28" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="E31" s="21">
         <v>0</v>
@@ -4318,13 +4314,13 @@
         <v>671800</v>
       </c>
       <c r="B32" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="D32" s="28" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="E32" s="21">
         <v>0</v>
@@ -4371,13 +4367,13 @@
         <v>671700</v>
       </c>
       <c r="B33" s="12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="D33" s="28" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="E33" s="21">
         <v>0</v>
@@ -4424,13 +4420,13 @@
         <v>671900</v>
       </c>
       <c r="B34" s="12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C34" s="12" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="D34" s="28" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="E34" s="21">
         <v>0</v>
@@ -4477,13 +4473,13 @@
         <v>672100</v>
       </c>
       <c r="B35" s="22" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="D35" s="28" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="E35" s="21">
         <v>0</v>
@@ -4530,13 +4526,13 @@
         <v>672260</v>
       </c>
       <c r="B36" s="22" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C36" s="12" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="D36" s="28" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="E36" s="21">
         <v>0</v>
@@ -4583,13 +4579,13 @@
         <v>671000</v>
       </c>
       <c r="B37" s="12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C37" s="12" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="D37" s="28" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="E37" s="21">
         <v>0</v>
@@ -4609,10 +4605,10 @@
         <v>Usage, Null, Null</v>
       </c>
       <c r="J37" s="20" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="K37" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="L37" s="18" t="str">
         <f>IF(AND(K37="Geschenk",Overview!E37=1,Overview!F37=0),'Logic ID'!$E$12,
@@ -4636,13 +4632,13 @@
         <v>671100</v>
       </c>
       <c r="B38" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="D38" s="28" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="E38" s="21">
         <v>0</v>
@@ -4662,10 +4658,10 @@
         <v>Usage, Null, Null</v>
       </c>
       <c r="J38" s="20" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="K38" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="L38" s="18" t="str">
         <f>IF(AND(K38="Geschenk",Overview!E38=1,Overview!F38=0),'Logic ID'!$E$12,
@@ -4689,13 +4685,13 @@
         <v>671200</v>
       </c>
       <c r="B39" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C39" s="12" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="D39" s="28" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="E39" s="21">
         <v>0</v>
@@ -4715,10 +4711,10 @@
         <v>Usage, Null, Null</v>
       </c>
       <c r="J39" s="20" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="K39" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="L39" s="18" t="str">
         <f>IF(AND(K39="Geschenk",Overview!E39=1,Overview!F39=0),'Logic ID'!$E$12,
@@ -4742,13 +4738,13 @@
         <v>671300</v>
       </c>
       <c r="B40" s="12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C40" s="12" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="D40" s="28" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="E40" s="21">
         <v>0</v>
@@ -4768,10 +4764,10 @@
         <v>Usage, Null, Null</v>
       </c>
       <c r="J40" s="20" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="K40" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="L40" s="18" t="str">
         <f>IF(AND(K40="Geschenk",Overview!E40=1,Overview!F40=0),'Logic ID'!$E$12,
@@ -4795,13 +4791,13 @@
         <v>671400</v>
       </c>
       <c r="B41" s="12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C41" s="12" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="D41" s="28" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="E41" s="21">
         <v>0</v>
@@ -4821,10 +4817,10 @@
         <v>Usage, Null, Null</v>
       </c>
       <c r="J41" s="20" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="K41" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="L41" s="18" t="str">
         <f>IF(AND(K41="Geschenk",Overview!E41=1,Overview!F41=0),'Logic ID'!$E$12,
@@ -4848,13 +4844,13 @@
         <v>671500</v>
       </c>
       <c r="B42" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C42" s="12" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="D42" s="28" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
       <c r="E42" s="21">
         <v>0</v>
@@ -4874,10 +4870,10 @@
         <v>Usage, Null, Null</v>
       </c>
       <c r="J42" s="20" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="K42" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="L42" s="18" t="str">
         <f>IF(AND(K42="Geschenk",Overview!E42=1,Overview!F42=0),'Logic ID'!$E$12,
@@ -4901,13 +4897,13 @@
         <v>613350</v>
       </c>
       <c r="B43" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="C43" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="C43" s="12" t="s">
-        <v>78</v>
-      </c>
       <c r="D43" s="28" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
       <c r="E43" s="21">
         <v>0</v>
@@ -4927,10 +4923,10 @@
         <v>Usage, Null, Null</v>
       </c>
       <c r="J43" s="20" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="K43" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="L43" s="18" t="str">
         <f>IF(AND(K43="Geschenk",Overview!E43=1,Overview!F43=0),'Logic ID'!$E$12,
@@ -4954,13 +4950,13 @@
         <v>661300</v>
       </c>
       <c r="B44" s="12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C44" s="12" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="D44" s="28" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
       <c r="E44" s="21">
         <v>0</v>
@@ -5007,13 +5003,13 @@
         <v>674300</v>
       </c>
       <c r="B45" s="12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C45" s="12" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="D45" s="28" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
       <c r="E45" s="21">
         <v>0</v>
@@ -5060,13 +5056,13 @@
         <v>605300</v>
       </c>
       <c r="B46" s="12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C46" s="12" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="D46" s="28" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="E46" s="17">
         <v>4</v>
@@ -5083,10 +5079,10 @@
       </c>
       <c r="I46" s="28" t="str">
         <f>VLOOKUP(L46,'Logic ID'!$E:$G,3,0)</f>
-        <v>Amount, Duration, Usage</v>
+        <v>Amount, Usage, Duration</v>
       </c>
       <c r="J46" s="13" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="K46" s="12" t="s">
         <v>17</v>
@@ -5113,13 +5109,13 @@
         <v>605300</v>
       </c>
       <c r="B47" s="12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C47" s="12" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="D47" s="28" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="E47" s="17">
         <v>4</v>
@@ -5136,10 +5132,10 @@
       </c>
       <c r="I47" s="28" t="str">
         <f>VLOOKUP(L47,'Logic ID'!$E:$G,3,0)</f>
-        <v>Amount, Duration, Usage</v>
+        <v>Amount, Usage, Duration</v>
       </c>
       <c r="J47" s="13" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="K47" s="12" t="s">
         <v>17</v>
@@ -5166,16 +5162,16 @@
         <v>605300</v>
       </c>
       <c r="B48" s="12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C48" s="12" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="D48" s="28" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="E48" s="21" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F48" s="17">
         <v>0</v>
@@ -5189,10 +5185,10 @@
       </c>
       <c r="I48" s="28" t="str">
         <f>VLOOKUP(L48,'Logic ID'!$E:$G,3,0)</f>
-        <v>Amount, Duration, Usage</v>
+        <v>Amount, Usage, Duration</v>
       </c>
       <c r="J48" s="13" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="K48" s="12" t="s">
         <v>17</v>
@@ -5219,13 +5215,13 @@
         <v>673901</v>
       </c>
       <c r="B49" s="12" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C49" s="12" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="D49" s="28" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
       <c r="E49" s="21">
         <v>0</v>
@@ -5272,13 +5268,13 @@
         <v>673902</v>
       </c>
       <c r="B50" s="23" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C50" s="12" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="D50" s="28" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
       <c r="E50" s="17">
         <v>4</v>
@@ -5295,10 +5291,10 @@
       </c>
       <c r="I50" s="28" t="str">
         <f>VLOOKUP(L50,'Logic ID'!$E:$G,3,0)</f>
-        <v>Amount, Duration, Usage</v>
+        <v>Amount, Usage, Duration</v>
       </c>
       <c r="J50" s="20" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K50" s="12" t="s">
         <v>46</v>
@@ -5325,13 +5321,13 @@
         <v>673902</v>
       </c>
       <c r="B51" s="23" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C51" s="12" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="D51" s="28" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
       <c r="E51" s="17">
         <v>0</v>
@@ -5348,10 +5344,10 @@
       </c>
       <c r="I51" s="28" t="str">
         <f>VLOOKUP(L51,'Logic ID'!$E:$G,3,0)</f>
-        <v>Amount, Duration, Usage</v>
+        <v>Amount, Usage, Duration</v>
       </c>
       <c r="J51" s="20" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K51" s="12" t="s">
         <v>46</v>
@@ -5378,13 +5374,13 @@
         <v>613300</v>
       </c>
       <c r="B52" s="24" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C52" s="12" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="D52" s="28" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="E52" s="21">
         <v>0</v>
@@ -5431,13 +5427,13 @@
         <v>691000</v>
       </c>
       <c r="B53" s="12" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C53" s="12" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="D53" s="28" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="E53" s="21">
         <v>0</v>
@@ -5460,7 +5456,7 @@
         <v>217</v>
       </c>
       <c r="K53" s="12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="L53" s="18" t="str">
         <f>IF(AND(K53="Geschenk",Overview!E53=1,Overview!F53=0),'Logic ID'!$E$12,
@@ -5484,13 +5480,13 @@
         <v>691100</v>
       </c>
       <c r="B54" s="12" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C54" s="12" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="D54" s="28" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="E54" s="21">
         <v>0</v>
@@ -5513,7 +5509,7 @@
         <v>217</v>
       </c>
       <c r="K54" s="12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="L54" s="18" t="str">
         <f>IF(AND(K54="Geschenk",Overview!E54=1,Overview!F54=0),'Logic ID'!$E$12,
@@ -5537,13 +5533,13 @@
         <v>691200</v>
       </c>
       <c r="B55" s="12" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C55" s="12" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="D55" s="28" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="E55" s="21">
         <v>0</v>
@@ -5566,7 +5562,7 @@
         <v>217</v>
       </c>
       <c r="K55" s="11" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="L55" s="18" t="str">
         <f>IF(AND(K55="Geschenk",Overview!E55=1,Overview!F55=0),'Logic ID'!$E$12,
@@ -5590,13 +5586,13 @@
         <v>691210</v>
       </c>
       <c r="B56" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="C56" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="C56" s="12" t="s">
-        <v>99</v>
-      </c>
       <c r="D56" s="28" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="E56" s="21">
         <v>0</v>
@@ -5619,7 +5615,7 @@
         <v>217</v>
       </c>
       <c r="K56" s="12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="L56" s="18" t="str">
         <f>IF(AND(K56="Geschenk",Overview!E56=1,Overview!F56=0),'Logic ID'!$E$12,
@@ -5643,13 +5639,13 @@
         <v>661711</v>
       </c>
       <c r="B57" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="C57" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="C57" s="12" t="s">
-        <v>101</v>
-      </c>
       <c r="D57" s="28" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="E57" s="21">
         <v>0</v>
@@ -5696,13 +5692,13 @@
         <v>673300</v>
       </c>
       <c r="B58" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="C58" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="C58" s="12" t="s">
-        <v>104</v>
-      </c>
       <c r="D58" s="28" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="E58" s="21">
         <v>0</v>
@@ -5722,7 +5718,7 @@
         <v>Usage, Null, Null</v>
       </c>
       <c r="J58" s="13" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="K58" s="12" t="s">
         <v>26</v>
@@ -5749,13 +5745,13 @@
         <v>673500</v>
       </c>
       <c r="B59" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="C59" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="C59" s="12" t="s">
-        <v>107</v>
-      </c>
       <c r="D59" s="28" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="E59" s="17">
         <v>4</v>
@@ -5772,10 +5768,10 @@
       </c>
       <c r="I59" s="28" t="str">
         <f>VLOOKUP(L59,'Logic ID'!$E:$G,3,0)</f>
-        <v>Amount, Duration, Usage</v>
+        <v>Amount, Usage, Duration</v>
       </c>
       <c r="J59" s="20" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K59" s="12" t="s">
         <v>46</v>
@@ -5802,13 +5798,13 @@
         <v>673500</v>
       </c>
       <c r="B60" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="C60" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="C60" s="12" t="s">
-        <v>107</v>
-      </c>
       <c r="D60" s="28" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="E60" s="17">
         <v>0</v>
@@ -5825,10 +5821,10 @@
       </c>
       <c r="I60" s="28" t="str">
         <f>VLOOKUP(L60,'Logic ID'!$E:$G,3,0)</f>
-        <v>Amount, Duration, Usage</v>
+        <v>Amount, Usage, Duration</v>
       </c>
       <c r="J60" s="20" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K60" s="12" t="s">
         <v>46</v>
@@ -5855,13 +5851,13 @@
         <v>673501</v>
       </c>
       <c r="B61" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="C61" s="12" t="s">
         <v>109</v>
       </c>
-      <c r="C61" s="12" t="s">
-        <v>110</v>
-      </c>
       <c r="D61" s="28" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="E61" s="21">
         <v>0</v>
@@ -5881,7 +5877,7 @@
         <v>Usage, Null, Null</v>
       </c>
       <c r="J61" s="13" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="K61" s="12" t="s">
         <v>26</v>
@@ -5908,13 +5904,13 @@
         <v>661000</v>
       </c>
       <c r="B62" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C62" s="12" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="D62" s="28" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="E62" s="21">
         <v>0</v>
@@ -5934,7 +5930,7 @@
         <v>Usage, Null, Null</v>
       </c>
       <c r="J62" s="13" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="K62" s="12" t="s">
         <v>26</v>
@@ -5961,13 +5957,13 @@
         <v>661400</v>
       </c>
       <c r="B63" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="C63" s="12" t="s">
         <v>113</v>
       </c>
-      <c r="C63" s="12" t="s">
-        <v>114</v>
-      </c>
-      <c r="D63" s="32" t="s">
-        <v>301</v>
+      <c r="D63" s="33" t="s">
+        <v>296</v>
       </c>
       <c r="E63" s="21">
         <v>0</v>
@@ -5987,7 +5983,7 @@
         <v>Usage, Null, Null</v>
       </c>
       <c r="J63" s="13" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="K63" s="12" t="s">
         <v>26</v>
@@ -6014,13 +6010,13 @@
         <v>661500</v>
       </c>
       <c r="B64" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="C64" s="12" t="s">
         <v>115</v>
       </c>
-      <c r="C64" s="12" t="s">
-        <v>116</v>
-      </c>
       <c r="D64" s="28" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="E64" s="21">
         <v>0</v>
@@ -6067,13 +6063,13 @@
         <v>671600</v>
       </c>
       <c r="B65" s="12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C65" s="12" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="D65" s="28" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="E65" s="21">
         <v>0</v>
@@ -6120,13 +6116,13 @@
         <v>673700</v>
       </c>
       <c r="B66" s="12" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C66" s="12" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="D66" s="28" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="E66" s="17">
         <v>4</v>
@@ -6143,10 +6139,10 @@
       </c>
       <c r="I66" s="28" t="str">
         <f>VLOOKUP(L66,'Logic ID'!$E:$G,3,0)</f>
-        <v>Amount, Duration, Usage</v>
+        <v>Amount, Usage, Duration</v>
       </c>
       <c r="J66" s="20" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K66" s="12" t="s">
         <v>46</v>
@@ -6173,13 +6169,13 @@
         <v>673700</v>
       </c>
       <c r="B67" s="12" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C67" s="12" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="D67" s="28" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="E67" s="17">
         <v>0</v>
@@ -6196,10 +6192,10 @@
       </c>
       <c r="I67" s="28" t="str">
         <f>VLOOKUP(L67,'Logic ID'!$E:$G,3,0)</f>
-        <v>Amount, Duration, Usage</v>
+        <v>Amount, Usage, Duration</v>
       </c>
       <c r="J67" s="20" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K67" s="12" t="s">
         <v>46</v>
@@ -6226,13 +6222,13 @@
         <v>674100</v>
       </c>
       <c r="B68" s="12" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C68" s="12" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="D68" s="28" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="E68" s="17">
         <v>4</v>
@@ -6249,10 +6245,10 @@
       </c>
       <c r="I68" s="28" t="str">
         <f>VLOOKUP(L68,'Logic ID'!$E:$G,3,0)</f>
-        <v>Amount, Duration, Usage</v>
+        <v>Amount, Usage, Duration</v>
       </c>
       <c r="J68" s="20" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K68" s="12" t="s">
         <v>46</v>
@@ -6279,13 +6275,13 @@
         <v>674100</v>
       </c>
       <c r="B69" s="12" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C69" s="12" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="D69" s="28" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="E69" s="17">
         <v>0</v>
@@ -6302,10 +6298,10 @@
       </c>
       <c r="I69" s="28" t="str">
         <f>VLOOKUP(L69,'Logic ID'!$E:$G,3,0)</f>
-        <v>Amount, Duration, Usage</v>
+        <v>Amount, Usage, Duration</v>
       </c>
       <c r="J69" s="20" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K69" s="12" t="s">
         <v>46</v>
@@ -6332,13 +6328,13 @@
         <v>674600</v>
       </c>
       <c r="B70" s="12" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C70" s="12" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="D70" s="28" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="E70" s="21">
         <v>0</v>
@@ -6358,7 +6354,7 @@
         <v>Usage, Null, Null</v>
       </c>
       <c r="J70" s="13" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="K70" s="12" t="s">
         <v>26</v>
@@ -6385,13 +6381,13 @@
         <v>605200</v>
       </c>
       <c r="B71" s="12" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C71" s="12" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="D71" s="28" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="E71" s="17">
         <v>4</v>
@@ -6408,10 +6404,10 @@
       </c>
       <c r="I71" s="28" t="str">
         <f>VLOOKUP(L71,'Logic ID'!$E:$G,3,0)</f>
-        <v>Amount, Duration, Usage</v>
+        <v>Amount, Usage, Duration</v>
       </c>
       <c r="J71" s="20" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="K71" s="12" t="s">
         <v>17</v>
@@ -6438,13 +6434,13 @@
         <v>605200</v>
       </c>
       <c r="B72" s="12" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C72" s="12" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="D72" s="28" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="E72" s="17">
         <v>4</v>
@@ -6461,10 +6457,10 @@
       </c>
       <c r="I72" s="28" t="str">
         <f>VLOOKUP(L72,'Logic ID'!$E:$G,3,0)</f>
-        <v>Amount, Duration, Usage</v>
+        <v>Amount, Usage, Duration</v>
       </c>
       <c r="J72" s="20" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="K72" s="12" t="s">
         <v>17</v>
@@ -6491,16 +6487,16 @@
         <v>605200</v>
       </c>
       <c r="B73" s="12" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C73" s="12" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="D73" s="28" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="E73" s="21" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F73" s="17">
         <v>0</v>
@@ -6514,10 +6510,10 @@
       </c>
       <c r="I73" s="28" t="str">
         <f>VLOOKUP(L73,'Logic ID'!$E:$G,3,0)</f>
-        <v>Amount, Duration, Usage</v>
+        <v>Amount, Usage, Duration</v>
       </c>
       <c r="J73" s="20" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="K73" s="12" t="s">
         <v>17</v>
@@ -6544,13 +6540,13 @@
         <v>681200</v>
       </c>
       <c r="B74" s="12" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C74" s="12" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="D74" s="28" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="E74" s="17">
         <v>4</v>
@@ -6567,10 +6563,10 @@
       </c>
       <c r="I74" s="28" t="str">
         <f>VLOOKUP(L74,'Logic ID'!$E:$G,3,0)</f>
-        <v>Amount, Duration, Usage</v>
+        <v>Amount, Usage, Duration</v>
       </c>
       <c r="J74" s="20" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K74" s="12" t="s">
         <v>46</v>
@@ -6597,13 +6593,13 @@
         <v>681200</v>
       </c>
       <c r="B75" s="12" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C75" s="12" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="D75" s="28" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="E75" s="17">
         <v>0</v>
@@ -6620,10 +6616,10 @@
       </c>
       <c r="I75" s="28" t="str">
         <f>VLOOKUP(L75,'Logic ID'!$E:$G,3,0)</f>
-        <v>Amount, Duration, Usage</v>
+        <v>Amount, Usage, Duration</v>
       </c>
       <c r="J75" s="20" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K75" s="12" t="s">
         <v>46</v>
@@ -6650,13 +6646,13 @@
         <v>603400</v>
       </c>
       <c r="B76" s="12" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C76" s="12" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="D76" s="28" t="s">
-        <v>349</v>
+        <v>361</v>
       </c>
       <c r="E76" s="17">
         <v>4</v>
@@ -6673,10 +6669,10 @@
       </c>
       <c r="I76" s="28" t="str">
         <f>VLOOKUP(L76,'Logic ID'!$E:$G,3,0)</f>
-        <v>Amount, Duration, Usage</v>
+        <v>Amount, Usage, Duration</v>
       </c>
       <c r="J76" s="20" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="K76" s="12" t="s">
         <v>17</v>
@@ -6703,13 +6699,13 @@
         <v>603400</v>
       </c>
       <c r="B77" s="12" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C77" s="12" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="D77" s="28" t="s">
-        <v>349</v>
+        <v>361</v>
       </c>
       <c r="E77" s="17">
         <v>4</v>
@@ -6726,10 +6722,10 @@
       </c>
       <c r="I77" s="28" t="str">
         <f>VLOOKUP(L77,'Logic ID'!$E:$G,3,0)</f>
-        <v>Amount, Duration, Usage</v>
+        <v>Amount, Usage, Duration</v>
       </c>
       <c r="J77" s="20" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="K77" s="12" t="s">
         <v>17</v>
@@ -6756,16 +6752,16 @@
         <v>603400</v>
       </c>
       <c r="B78" s="12" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C78" s="12" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="D78" s="28" t="s">
-        <v>349</v>
+        <v>361</v>
       </c>
       <c r="E78" s="21" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F78" s="17">
         <v>0</v>
@@ -6779,10 +6775,10 @@
       </c>
       <c r="I78" s="28" t="str">
         <f>VLOOKUP(L78,'Logic ID'!$E:$G,3,0)</f>
-        <v>Amount, Duration, Usage</v>
+        <v>Amount, Usage, Duration</v>
       </c>
       <c r="J78" s="20" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="K78" s="12" t="s">
         <v>17</v>
@@ -6809,13 +6805,13 @@
         <v>605210</v>
       </c>
       <c r="B79" s="12" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C79" s="12" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="D79" s="28" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="E79" s="17">
         <v>4</v>
@@ -6832,10 +6828,10 @@
       </c>
       <c r="I79" s="28" t="str">
         <f>VLOOKUP(L79,'Logic ID'!$E:$G,3,0)</f>
-        <v>Amount, Duration, Usage</v>
+        <v>Amount, Usage, Duration</v>
       </c>
       <c r="J79" s="20" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="K79" s="12" t="s">
         <v>17</v>
@@ -6862,13 +6858,13 @@
         <v>605210</v>
       </c>
       <c r="B80" s="12" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C80" s="12" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="D80" s="28" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="E80" s="17">
         <v>4</v>
@@ -6885,10 +6881,10 @@
       </c>
       <c r="I80" s="28" t="str">
         <f>VLOOKUP(L80,'Logic ID'!$E:$G,3,0)</f>
-        <v>Amount, Duration, Usage</v>
+        <v>Amount, Usage, Duration</v>
       </c>
       <c r="J80" s="20" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="K80" s="12" t="s">
         <v>17</v>
@@ -6915,16 +6911,16 @@
         <v>605210</v>
       </c>
       <c r="B81" s="12" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C81" s="12" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="D81" s="28" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="E81" s="21" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F81" s="17">
         <v>0</v>
@@ -6938,10 +6934,10 @@
       </c>
       <c r="I81" s="28" t="str">
         <f>VLOOKUP(L81,'Logic ID'!$E:$G,3,0)</f>
-        <v>Amount, Duration, Usage</v>
+        <v>Amount, Usage, Duration</v>
       </c>
       <c r="J81" s="20" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="K81" s="12" t="s">
         <v>17</v>
@@ -6968,13 +6964,13 @@
         <v>673200</v>
       </c>
       <c r="B82" s="12" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C82" s="12" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="D82" s="28" t="s">
-        <v>351</v>
+        <v>345</v>
       </c>
       <c r="E82" s="21">
         <v>0</v>
@@ -6994,7 +6990,7 @@
         <v>Usage, Null, Null</v>
       </c>
       <c r="J82" s="13" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="K82" s="11" t="s">
         <v>26</v>
@@ -7021,13 +7017,13 @@
         <v>673400</v>
       </c>
       <c r="B83" s="12" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C83" s="12" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="D83" s="28" t="s">
-        <v>352</v>
+        <v>346</v>
       </c>
       <c r="E83" s="21">
         <v>0</v>
@@ -7047,7 +7043,7 @@
         <v>Usage, Null, Null</v>
       </c>
       <c r="J83" s="13" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="K83" s="11" t="s">
         <v>26</v>
@@ -7074,13 +7070,13 @@
         <v>695300</v>
       </c>
       <c r="B84" s="12" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C84" s="12" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="D84" s="28" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="E84" s="21">
         <v>0</v>
@@ -7127,13 +7123,13 @@
         <v>695400</v>
       </c>
       <c r="B85" s="12" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C85" s="12" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="D85" s="28" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="E85" s="17">
         <v>4</v>
@@ -7150,10 +7146,10 @@
       </c>
       <c r="I85" s="28" t="str">
         <f>VLOOKUP(L85,'Logic ID'!$E:$G,3,0)</f>
-        <v>Amount, Duration, Usage</v>
+        <v>Amount, Usage, Duration</v>
       </c>
       <c r="J85" s="20" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="K85" s="12" t="s">
         <v>17</v>
@@ -7180,13 +7176,13 @@
         <v>695400</v>
       </c>
       <c r="B86" s="12" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C86" s="12" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="D86" s="28" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="E86" s="17">
         <v>4</v>
@@ -7203,10 +7199,10 @@
       </c>
       <c r="I86" s="28" t="str">
         <f>VLOOKUP(L86,'Logic ID'!$E:$G,3,0)</f>
-        <v>Amount, Duration, Usage</v>
+        <v>Amount, Usage, Duration</v>
       </c>
       <c r="J86" s="20" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="K86" s="12" t="s">
         <v>17</v>
@@ -7233,16 +7229,16 @@
         <v>695400</v>
       </c>
       <c r="B87" s="12" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C87" s="12" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="D87" s="28" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="E87" s="21" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F87" s="17">
         <v>0</v>
@@ -7256,10 +7252,10 @@
       </c>
       <c r="I87" s="28" t="str">
         <f>VLOOKUP(L87,'Logic ID'!$E:$G,3,0)</f>
-        <v>Amount, Duration, Usage</v>
+        <v>Amount, Usage, Duration</v>
       </c>
       <c r="J87" s="20" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="K87" s="12" t="s">
         <v>17</v>
@@ -7286,13 +7282,13 @@
         <v>605100</v>
       </c>
       <c r="B88" s="12" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C88" s="12" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="D88" s="28" t="s">
-        <v>343</v>
+        <v>360</v>
       </c>
       <c r="E88" s="17">
         <v>4</v>
@@ -7309,10 +7305,10 @@
       </c>
       <c r="I88" s="28" t="str">
         <f>VLOOKUP(L88,'Logic ID'!$E:$G,3,0)</f>
-        <v>Amount, Duration, Usage</v>
+        <v>Amount, Usage, Duration</v>
       </c>
       <c r="J88" s="20" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="K88" s="12" t="s">
         <v>17</v>
@@ -7339,13 +7335,13 @@
         <v>605100</v>
       </c>
       <c r="B89" s="12" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C89" s="12" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="D89" s="28" t="s">
-        <v>343</v>
+        <v>360</v>
       </c>
       <c r="E89" s="17">
         <v>4</v>
@@ -7362,10 +7358,10 @@
       </c>
       <c r="I89" s="28" t="str">
         <f>VLOOKUP(L89,'Logic ID'!$E:$G,3,0)</f>
-        <v>Amount, Duration, Usage</v>
+        <v>Amount, Usage, Duration</v>
       </c>
       <c r="J89" s="20" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="K89" s="12" t="s">
         <v>17</v>
@@ -7392,16 +7388,16 @@
         <v>605100</v>
       </c>
       <c r="B90" s="12" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C90" s="12" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="D90" s="28" t="s">
-        <v>343</v>
+        <v>360</v>
       </c>
       <c r="E90" s="21" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F90" s="17">
         <v>0</v>
@@ -7415,10 +7411,10 @@
       </c>
       <c r="I90" s="28" t="str">
         <f>VLOOKUP(L90,'Logic ID'!$E:$G,3,0)</f>
-        <v>Amount, Duration, Usage</v>
+        <v>Amount, Usage, Duration</v>
       </c>
       <c r="J90" s="20" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="K90" s="12" t="s">
         <v>17</v>
@@ -7445,13 +7441,13 @@
         <v>674400</v>
       </c>
       <c r="B91" s="12" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C91" s="12" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="D91" s="28" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="E91" s="17">
         <v>4</v>
@@ -7468,10 +7464,10 @@
       </c>
       <c r="I91" s="28" t="str">
         <f>VLOOKUP(L91,'Logic ID'!$E:$G,3,0)</f>
-        <v>Amount, Duration, Usage</v>
+        <v>Amount, Usage, Duration</v>
       </c>
       <c r="J91" s="13" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K91" s="12" t="s">
         <v>46</v>
@@ -7498,13 +7494,13 @@
         <v>674400</v>
       </c>
       <c r="B92" s="12" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C92" s="12" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="D92" s="28" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="E92" s="17">
         <v>0</v>
@@ -7521,10 +7517,10 @@
       </c>
       <c r="I92" s="28" t="str">
         <f>VLOOKUP(L92,'Logic ID'!$E:$G,3,0)</f>
-        <v>Amount, Duration, Usage</v>
+        <v>Amount, Usage, Duration</v>
       </c>
       <c r="J92" s="13" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K92" s="12" t="s">
         <v>46</v>
@@ -7551,13 +7547,13 @@
         <v>607700</v>
       </c>
       <c r="B93" s="12" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C93" s="12" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="D93" s="28" t="s">
-        <v>355</v>
+        <v>349</v>
       </c>
       <c r="E93" s="21">
         <v>0</v>
@@ -7604,13 +7600,13 @@
         <v>608030</v>
       </c>
       <c r="B94" s="12" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C94" s="12" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="D94" s="28" t="s">
-        <v>355</v>
+        <v>349</v>
       </c>
       <c r="E94" s="21">
         <v>0</v>
@@ -7657,13 +7653,13 @@
         <v>605400</v>
       </c>
       <c r="B95" s="12" t="s">
+        <v>145</v>
+      </c>
+      <c r="C95" s="12" t="s">
         <v>146</v>
       </c>
-      <c r="C95" s="12" t="s">
-        <v>147</v>
-      </c>
-      <c r="D95" s="32" t="s">
-        <v>301</v>
+      <c r="D95" s="33" t="s">
+        <v>296</v>
       </c>
       <c r="E95" s="21">
         <v>0</v>
@@ -7683,7 +7679,7 @@
         <v>Usage, Null, Null</v>
       </c>
       <c r="J95" s="20" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="K95" s="12" t="s">
         <v>26</v>
@@ -7710,13 +7706,13 @@
         <v>694900</v>
       </c>
       <c r="B96" s="12" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C96" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="D96" s="32" t="s">
-        <v>301</v>
+        <v>147</v>
+      </c>
+      <c r="D96" s="33" t="s">
+        <v>296</v>
       </c>
       <c r="E96" s="21">
         <v>0</v>
@@ -7763,13 +7759,13 @@
         <v>695000</v>
       </c>
       <c r="B97" s="12" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C97" s="12" t="s">
-        <v>149</v>
-      </c>
-      <c r="D97" s="32" t="s">
-        <v>301</v>
+        <v>148</v>
+      </c>
+      <c r="D97" s="33" t="s">
+        <v>296</v>
       </c>
       <c r="E97" s="21">
         <v>0</v>
@@ -7816,13 +7812,13 @@
         <v>695100</v>
       </c>
       <c r="B98" s="12" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C98" s="12" t="s">
-        <v>284</v>
-      </c>
-      <c r="D98" s="32" t="s">
-        <v>301</v>
+        <v>279</v>
+      </c>
+      <c r="D98" s="33" t="s">
+        <v>296</v>
       </c>
       <c r="E98" s="21">
         <v>0</v>
@@ -7869,13 +7865,13 @@
         <v>695200</v>
       </c>
       <c r="B99" s="12" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C99" s="12" t="s">
-        <v>151</v>
-      </c>
-      <c r="D99" s="32" t="s">
-        <v>301</v>
+        <v>150</v>
+      </c>
+      <c r="D99" s="33" t="s">
+        <v>296</v>
       </c>
       <c r="E99" s="21">
         <v>0</v>
@@ -7922,13 +7918,13 @@
         <v>673600</v>
       </c>
       <c r="B100" s="12" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C100" s="12" t="s">
-        <v>285</v>
-      </c>
-      <c r="D100" s="32" t="s">
-        <v>301</v>
+        <v>280</v>
+      </c>
+      <c r="D100" s="33" t="s">
+        <v>296</v>
       </c>
       <c r="E100" s="21">
         <v>0</v>
@@ -7975,13 +7971,13 @@
         <v>662400</v>
       </c>
       <c r="B101" s="12" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C101" s="12" t="s">
-        <v>286</v>
-      </c>
-      <c r="D101" s="32" t="s">
-        <v>301</v>
+        <v>281</v>
+      </c>
+      <c r="D101" s="33" t="s">
+        <v>296</v>
       </c>
       <c r="E101" s="21">
         <v>0</v>
@@ -8028,13 +8024,13 @@
         <v>662500</v>
       </c>
       <c r="B102" s="12" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C102" s="12" t="s">
-        <v>287</v>
-      </c>
-      <c r="D102" s="32" t="s">
-        <v>301</v>
+        <v>282</v>
+      </c>
+      <c r="D102" s="33" t="s">
+        <v>296</v>
       </c>
       <c r="E102" s="21">
         <v>0</v>
@@ -8081,13 +8077,13 @@
         <v>672310</v>
       </c>
       <c r="B103" s="12" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C103" s="12" t="s">
-        <v>288</v>
-      </c>
-      <c r="D103" s="32" t="s">
-        <v>301</v>
+        <v>283</v>
+      </c>
+      <c r="D103" s="33" t="s">
+        <v>296</v>
       </c>
       <c r="E103" s="21">
         <v>0</v>
@@ -8134,13 +8130,13 @@
         <v>672320</v>
       </c>
       <c r="B104" s="12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C104" s="12" t="s">
-        <v>289</v>
-      </c>
-      <c r="D104" s="32" t="s">
-        <v>301</v>
+        <v>284</v>
+      </c>
+      <c r="D104" s="33" t="s">
+        <v>296</v>
       </c>
       <c r="E104" s="21">
         <v>0</v>
@@ -8187,13 +8183,13 @@
         <v>672400</v>
       </c>
       <c r="B105" s="12" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C105" s="12" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="D105" s="28" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
       <c r="E105" s="21">
         <v>0</v>
@@ -8240,13 +8236,13 @@
         <v>672500</v>
       </c>
       <c r="B106" s="12" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C106" s="12" t="s">
-        <v>291</v>
-      </c>
-      <c r="D106" s="32" t="s">
-        <v>301</v>
+        <v>286</v>
+      </c>
+      <c r="D106" s="33" t="s">
+        <v>296</v>
       </c>
       <c r="E106" s="21">
         <v>0</v>
@@ -8293,13 +8289,13 @@
         <v>672600</v>
       </c>
       <c r="B107" s="12" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C107" s="12" t="s">
-        <v>292</v>
-      </c>
-      <c r="D107" s="32" t="s">
-        <v>301</v>
+        <v>287</v>
+      </c>
+      <c r="D107" s="33" t="s">
+        <v>296</v>
       </c>
       <c r="E107" s="21">
         <v>0</v>
@@ -8346,13 +8342,13 @@
         <v>672700</v>
       </c>
       <c r="B108" s="12" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C108" s="12" t="s">
-        <v>293</v>
-      </c>
-      <c r="D108" s="32" t="s">
-        <v>301</v>
+        <v>288</v>
+      </c>
+      <c r="D108" s="33" t="s">
+        <v>296</v>
       </c>
       <c r="E108" s="21">
         <v>0</v>
@@ -8399,13 +8395,13 @@
         <v>604400</v>
       </c>
       <c r="B109" s="12" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C109" s="12" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="D109" s="28" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="E109" s="21">
         <v>0</v>
@@ -8428,7 +8424,7 @@
         <v>217</v>
       </c>
       <c r="K109" s="12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="L109" s="18" t="str">
         <f>IF(AND(K109="Geschenk",Overview!E109=1,Overview!F109=0),'Logic ID'!$E$12,
@@ -8452,13 +8448,13 @@
         <v>604300</v>
       </c>
       <c r="B110" s="12" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C110" s="12" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="D110" s="28" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="E110" s="21">
         <v>0</v>
@@ -8481,7 +8477,7 @@
         <v>217</v>
       </c>
       <c r="K110" s="12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="L110" s="18" t="str">
         <f>IF(AND(K110="Geschenk",Overview!E110=1,Overview!F110=0),'Logic ID'!$E$12,
@@ -8505,13 +8501,13 @@
         <v>604310</v>
       </c>
       <c r="B111" s="12" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C111" s="12" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="D111" s="28" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="E111" s="21">
         <v>0</v>
@@ -8534,7 +8530,7 @@
         <v>217</v>
       </c>
       <c r="K111" s="12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="L111" s="18" t="str">
         <f>IF(AND(K111="Geschenk",Overview!E111=1,Overview!F111=0),'Logic ID'!$E$12,
@@ -8558,13 +8554,13 @@
         <v>604000</v>
       </c>
       <c r="B112" s="12" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C112" s="12" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="D112" s="28" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E112" s="21">
         <v>0</v>
@@ -8587,7 +8583,7 @@
         <v>217</v>
       </c>
       <c r="K112" s="12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="L112" s="18" t="str">
         <f>IF(AND(K112="Geschenk",Overview!E112=1,Overview!F112=0),'Logic ID'!$E$12,
@@ -8611,13 +8607,13 @@
         <v>691300</v>
       </c>
       <c r="B113" s="12" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C113" s="12" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="D113" s="28" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="E113" s="21">
         <v>0</v>
@@ -8640,7 +8636,7 @@
         <v>217</v>
       </c>
       <c r="K113" s="12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="L113" s="18" t="str">
         <f>IF(AND(K113="Geschenk",Overview!E113=1,Overview!F113=0),'Logic ID'!$E$12,
@@ -8664,13 +8660,13 @@
         <v>691310</v>
       </c>
       <c r="B114" s="12" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C114" s="12" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="D114" s="28" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="E114" s="21">
         <v>0</v>
@@ -8693,7 +8689,7 @@
         <v>217</v>
       </c>
       <c r="K114" s="12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="L114" s="18" t="str">
         <f>IF(AND(K114="Geschenk",Overview!E114=1,Overview!F114=0),'Logic ID'!$E$12,
@@ -8717,13 +8713,13 @@
         <v>691350</v>
       </c>
       <c r="B115" s="12" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C115" s="12" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="D115" s="28" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="E115" s="21">
         <v>0</v>
@@ -8746,7 +8742,7 @@
         <v>217</v>
       </c>
       <c r="K115" s="12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="L115" s="18" t="str">
         <f>IF(AND(K115="Geschenk",Overview!E115=1,Overview!F115=0),'Logic ID'!$E$12,
@@ -8770,13 +8766,13 @@
         <v>661150</v>
       </c>
       <c r="B116" s="12" t="s">
+        <v>167</v>
+      </c>
+      <c r="C116" s="12" t="s">
         <v>168</v>
       </c>
-      <c r="C116" s="12" t="s">
-        <v>169</v>
-      </c>
-      <c r="D116" s="32" t="s">
-        <v>301</v>
+      <c r="D116" s="33" t="s">
+        <v>296</v>
       </c>
       <c r="E116" s="21">
         <v>0</v>
@@ -8823,13 +8819,13 @@
         <v>999910</v>
       </c>
       <c r="B117" s="12" t="s">
+        <v>169</v>
+      </c>
+      <c r="C117" s="12" t="s">
         <v>170</v>
       </c>
-      <c r="C117" s="12" t="s">
-        <v>171</v>
-      </c>
-      <c r="D117" s="32" t="s">
-        <v>301</v>
+      <c r="D117" s="33" t="s">
+        <v>296</v>
       </c>
       <c r="E117" s="21">
         <v>0</v>
@@ -8849,7 +8845,7 @@
         <v>Usage, Null, Null</v>
       </c>
       <c r="J117" s="20" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="K117" s="12" t="s">
         <v>26</v>
@@ -8904,10 +8900,10 @@
   <sheetData>
     <row r="1" spans="1:256" ht="14.45" customHeight="1">
       <c r="A1" s="10" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C1" s="10"/>
       <c r="D1" s="10"/>
@@ -9169,7 +9165,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -9194,7 +9190,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
@@ -9219,7 +9215,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
@@ -9244,7 +9240,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
@@ -9269,7 +9265,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
@@ -9441,10 +9437,10 @@
   <sheetData>
     <row r="1" spans="1:256" ht="14.45" customHeight="1">
       <c r="A1" s="10" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C1" s="10"/>
       <c r="D1" s="10"/>
@@ -9706,7 +9702,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -9729,7 +9725,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
@@ -9752,7 +9748,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
@@ -9919,7 +9915,7 @@
   <dimension ref="A1:IQ91"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="B48" sqref="B48"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.45" customHeight="1"/>
@@ -9931,10 +9927,10 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.45" customHeight="1">
@@ -10078,7 +10074,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>49</v>
+        <v>362</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="17.45" customHeight="1">
@@ -10086,7 +10082,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="17.45" customHeight="1">
@@ -10094,7 +10090,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="17.45" customHeight="1">
@@ -10102,7 +10098,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="17.45" customHeight="1">
@@ -10110,7 +10106,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="17.45" customHeight="1">
@@ -10118,7 +10114,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="17.45" customHeight="1">
@@ -10126,7 +10122,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="17.45" customHeight="1">
@@ -10134,7 +10130,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="17.45" customHeight="1">
@@ -10142,7 +10138,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="17.45" customHeight="1">
@@ -10150,7 +10146,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="17.45" customHeight="1">
@@ -10158,7 +10154,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="17.45" customHeight="1">
@@ -10166,7 +10162,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="17.45" customHeight="1">
@@ -10174,7 +10170,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="17.45" customHeight="1">
@@ -10182,7 +10178,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="17.45" customHeight="1">
@@ -10190,7 +10186,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="17.45" customHeight="1">
@@ -10198,7 +10194,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="17.45" customHeight="1">
@@ -10206,7 +10202,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="17.45" customHeight="1">
@@ -10214,7 +10210,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="17.45" customHeight="1">
@@ -10222,7 +10218,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="17.45" customHeight="1">
@@ -10230,7 +10226,7 @@
         <v>37</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="17.45" customHeight="1">
@@ -10238,7 +10234,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="18" customHeight="1">
@@ -10246,7 +10242,7 @@
         <v>39</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="17.45" customHeight="1">
@@ -10254,7 +10250,7 @@
         <v>40</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="17.45" customHeight="1">
@@ -10262,7 +10258,7 @@
         <v>41</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="17.45" customHeight="1">
@@ -10270,7 +10266,7 @@
         <v>42</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="17.45" customHeight="1">
@@ -10278,7 +10274,7 @@
         <v>43</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="17.45" customHeight="1">
@@ -10286,7 +10282,7 @@
         <v>44</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="17.45" customHeight="1">
@@ -10294,7 +10290,7 @@
         <v>45</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="17.45" customHeight="1">
@@ -10302,7 +10298,7 @@
         <v>46</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="17.45" customHeight="1">
@@ -10310,7 +10306,7 @@
         <v>47</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="17.45" customHeight="1">
@@ -10318,7 +10314,7 @@
         <v>48</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="17.45" customHeight="1">
@@ -10326,7 +10322,7 @@
         <v>49</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="17.45" customHeight="1">
@@ -10334,7 +10330,7 @@
         <v>50</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="17.45" customHeight="1">
@@ -10342,7 +10338,7 @@
         <v>51</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="17.45" customHeight="1">
@@ -10350,7 +10346,7 @@
         <v>52</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="17.45" customHeight="1">
@@ -10358,7 +10354,7 @@
         <v>53</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="17.45" customHeight="1">
@@ -10366,7 +10362,7 @@
         <v>54</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="17.45" customHeight="1">
@@ -10374,7 +10370,7 @@
         <v>55</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="17.45" customHeight="1">
@@ -10382,7 +10378,7 @@
         <v>56</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="17.45" customHeight="1">
@@ -10390,7 +10386,7 @@
         <v>57</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="17.45" customHeight="1">
@@ -10398,7 +10394,7 @@
         <v>58</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="17.45" customHeight="1">
@@ -10406,7 +10402,7 @@
         <v>59</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="17.45" customHeight="1">
@@ -10414,7 +10410,7 @@
         <v>60</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="17.45" customHeight="1">
@@ -10422,7 +10418,7 @@
         <v>61</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="17.45" customHeight="1">
@@ -10430,7 +10426,7 @@
         <v>62</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="17.45" customHeight="1">
@@ -10438,7 +10434,7 @@
         <v>63</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="17.45" customHeight="1">
@@ -10446,7 +10442,7 @@
         <v>64</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="17.45" customHeight="1">
@@ -10454,7 +10450,7 @@
         <v>65</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="17.45" customHeight="1">
@@ -10462,7 +10458,7 @@
         <v>66</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="17.45" customHeight="1">
@@ -10470,7 +10466,7 @@
         <v>67</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="17.45" customHeight="1">
@@ -10478,7 +10474,7 @@
         <v>68</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="17.45" customHeight="1">
@@ -10486,7 +10482,7 @@
         <v>69</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="17.45" customHeight="1">
@@ -10494,7 +10490,7 @@
         <v>70</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="17.45" customHeight="1">
@@ -10502,7 +10498,7 @@
         <v>71</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="17.45" customHeight="1">
@@ -10510,7 +10506,7 @@
         <v>72</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="17.45" customHeight="1">
@@ -10518,7 +10514,7 @@
         <v>73</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="17.45" customHeight="1">
@@ -10526,7 +10522,7 @@
         <v>74</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="76" spans="1:2" ht="17.45" customHeight="1">
@@ -10534,7 +10530,7 @@
         <v>75</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="17.45" customHeight="1">
@@ -10542,7 +10538,7 @@
         <v>76</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="17.45" customHeight="1">
@@ -10550,7 +10546,7 @@
         <v>77</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="79" spans="1:2" ht="17.45" customHeight="1">
@@ -10558,7 +10554,7 @@
         <v>78</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="80" spans="1:2" ht="17.45" customHeight="1">
@@ -10566,7 +10562,7 @@
         <v>79</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="17.45" customHeight="1">
@@ -10574,7 +10570,7 @@
         <v>80</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="82" spans="1:2" ht="17.45" customHeight="1">
@@ -10582,7 +10578,7 @@
         <v>81</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="17.45" customHeight="1">
@@ -10590,7 +10586,7 @@
         <v>82</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="84" spans="1:2" ht="17.45" customHeight="1">
@@ -10598,7 +10594,7 @@
         <v>83</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="85" spans="1:2" ht="17.45" customHeight="1">
@@ -10606,7 +10602,7 @@
         <v>84</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="86" spans="1:2" ht="17.45" customHeight="1">
@@ -10614,7 +10610,7 @@
         <v>85</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="87" spans="1:2" ht="17.45" customHeight="1">
@@ -10622,7 +10618,7 @@
         <v>86</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="88" spans="1:2" ht="17.45" customHeight="1">
@@ -10630,7 +10626,7 @@
         <v>87</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="89" spans="1:2" ht="17.45" customHeight="1">
@@ -10638,7 +10634,7 @@
         <v>88</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="17.45" customHeight="1">
@@ -10646,7 +10642,7 @@
         <v>89</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="17.45" customHeight="1">
@@ -10654,7 +10650,7 @@
         <v>90</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
   </sheetData>
@@ -10682,15 +10678,15 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>8</v>
@@ -10698,7 +10694,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>221</v>
@@ -10706,15 +10702,15 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>222</v>
@@ -10722,10 +10718,10 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -10796,7 +10792,7 @@
   <dimension ref="A1:IW24"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.45" customHeight="1"/>
@@ -10820,16 +10816,16 @@
         <v>3</v>
       </c>
       <c r="D1" s="31" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E1" s="31" t="s">
+        <v>205</v>
+      </c>
+      <c r="F1" s="31" t="s">
+        <v>180</v>
+      </c>
+      <c r="G1" s="31" t="s">
         <v>206</v>
-      </c>
-      <c r="F1" s="31" t="s">
-        <v>181</v>
-      </c>
-      <c r="G1" s="31" t="s">
-        <v>207</v>
       </c>
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
@@ -10867,7 +10863,7 @@
         <v>0</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
@@ -10899,13 +10895,13 @@
         <v>2</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="G3" s="33" t="s">
-        <v>361</v>
+        <v>181</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>213</v>
       </c>
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
@@ -10937,13 +10933,13 @@
         <v>1</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G4" s="33" t="s">
-        <v>361</v>
+      <c r="G4" s="1" t="s">
+        <v>213</v>
       </c>
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
@@ -10969,19 +10965,19 @@
         <v>17</v>
       </c>
       <c r="C5" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="D5" s="2">
-        <v>0</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="G5" s="33" t="s">
-        <v>361</v>
+      <c r="G5" s="32" t="s">
+        <v>213</v>
       </c>
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
@@ -11019,7 +11015,7 @@
         <v>0</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
@@ -11051,13 +11047,13 @@
         <v>2</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="G7" s="33" t="s">
-        <v>361</v>
+        <v>184</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>213</v>
       </c>
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
@@ -11089,13 +11085,13 @@
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G8" s="33" t="s">
-        <v>361</v>
+      <c r="G8" s="32" t="s">
+        <v>213</v>
       </c>
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
@@ -11118,7 +11114,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C9" s="2">
         <v>0</v>
@@ -11127,13 +11123,13 @@
         <v>0</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
@@ -11156,7 +11152,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C10" s="2">
         <v>0</v>
@@ -11165,13 +11161,13 @@
         <v>0</v>
       </c>
       <c r="E10" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="F10" s="1" t="s">
-        <v>188</v>
-      </c>
       <c r="G10" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
@@ -11194,7 +11190,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C11" s="2">
         <v>0</v>
@@ -11203,13 +11199,13 @@
         <v>0</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>0</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
@@ -11241,13 +11237,13 @@
         <v>0</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>0</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
@@ -11279,13 +11275,13 @@
         <v>0</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>0</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
@@ -11317,13 +11313,13 @@
         <v>0</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>0</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
@@ -14099,15 +14095,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxKeywordTaxHTField xmlns="45be70f0-66b9-4629-a389-4b080fc0dfa6">
@@ -14155,6 +14142,15 @@
 </p:properties>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{47BF3E90-0828-4759-ACA7-3670C46D50E8}">
   <ds:schemaRefs>
@@ -14175,14 +14171,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DC021B46-1420-4ED7-AC55-8BF0CD9341B9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4141748-E8CF-4376-BEDF-0CE4C9A34F7B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -14190,4 +14178,12 @@
     <ds:schemaRef ds:uri="45be70f0-66b9-4629-a389-4b080fc0dfa6"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DC021B46-1420-4ED7-AC55-8BF0CD9341B9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>